<commit_message>
Load input files as strings
</commit_message>
<xml_diff>
--- a/Input Files/Pole Book STEEL_MATCHED.xlsx
+++ b/Input Files/Pole Book STEEL_MATCHED.xlsx
@@ -731,7 +731,7 @@
       <c r="B10" s="2" t="inlineStr"/>
       <c r="C10" s="1" t="inlineStr">
         <is>
-          <t>01/Jun/2025</t>
+          <t>2025-06-01 00:00:00</t>
         </is>
       </c>
       <c r="D10" s="1" t="inlineStr">
@@ -748,8 +748,10 @@
       <c r="G10" s="1" t="inlineStr"/>
       <c r="H10" s="1" t="inlineStr"/>
       <c r="I10" s="1" t="inlineStr"/>
-      <c r="J10" s="7" t="n">
-        <v>3705637830.65</v>
+      <c r="J10" s="7" t="inlineStr">
+        <is>
+          <t>3705637830.65</t>
+        </is>
       </c>
       <c r="K10" s="1" t="inlineStr"/>
       <c r="L10" s="1" t="inlineStr"/>
@@ -759,7 +761,7 @@
       <c r="B11" s="2" t="inlineStr"/>
       <c r="C11" s="1" t="inlineStr">
         <is>
-          <t>01/Jun/2025</t>
+          <t>2025-06-01 00:00:00</t>
         </is>
       </c>
       <c r="D11" s="1" t="inlineStr">
@@ -785,8 +787,10 @@
         </is>
       </c>
       <c r="J11" s="1" t="inlineStr"/>
-      <c r="K11" s="7" t="n">
-        <v>6957</v>
+      <c r="K11" s="7" t="inlineStr">
+        <is>
+          <t>6957</t>
+        </is>
       </c>
       <c r="L11" s="1" t="inlineStr"/>
     </row>
@@ -835,7 +839,7 @@
       <c r="B14" s="2" t="inlineStr"/>
       <c r="C14" s="1" t="inlineStr">
         <is>
-          <t>01/Jun/2025</t>
+          <t>2025-06-01 00:00:00</t>
         </is>
       </c>
       <c r="D14" s="1" t="inlineStr">
@@ -861,8 +865,10 @@
         </is>
       </c>
       <c r="J14" s="1" t="inlineStr"/>
-      <c r="K14" s="7" t="n">
-        <v>8084</v>
+      <c r="K14" s="7" t="inlineStr">
+        <is>
+          <t>8084</t>
+        </is>
       </c>
       <c r="L14" s="1" t="inlineStr"/>
     </row>
@@ -911,7 +917,7 @@
       <c r="B17" s="2" t="inlineStr"/>
       <c r="C17" s="1" t="inlineStr">
         <is>
-          <t>01/Jun/2025</t>
+          <t>2025-06-01 00:00:00</t>
         </is>
       </c>
       <c r="D17" s="1" t="inlineStr">
@@ -937,8 +943,10 @@
         </is>
       </c>
       <c r="J17" s="1" t="inlineStr"/>
-      <c r="K17" s="7" t="n">
-        <v>5417</v>
+      <c r="K17" s="7" t="inlineStr">
+        <is>
+          <t>5417</t>
+        </is>
       </c>
       <c r="L17" s="1" t="inlineStr"/>
     </row>
@@ -987,7 +995,7 @@
       <c r="B20" s="2" t="inlineStr"/>
       <c r="C20" s="1" t="inlineStr">
         <is>
-          <t>01/Jun/2025</t>
+          <t>2025-06-01 00:00:00</t>
         </is>
       </c>
       <c r="D20" s="1" t="inlineStr">
@@ -1013,8 +1021,10 @@
         </is>
       </c>
       <c r="J20" s="1" t="inlineStr"/>
-      <c r="K20" s="7" t="n">
-        <v>2729</v>
+      <c r="K20" s="7" t="inlineStr">
+        <is>
+          <t>2729</t>
+        </is>
       </c>
       <c r="L20" s="1" t="inlineStr"/>
     </row>
@@ -1063,7 +1073,7 @@
       <c r="B23" s="2" t="inlineStr"/>
       <c r="C23" s="1" t="inlineStr">
         <is>
-          <t>01/Jun/2025</t>
+          <t>2025-06-01 00:00:00</t>
         </is>
       </c>
       <c r="D23" s="1" t="inlineStr">
@@ -1089,8 +1099,10 @@
         </is>
       </c>
       <c r="J23" s="1" t="inlineStr"/>
-      <c r="K23" s="7" t="n">
-        <v>26500</v>
+      <c r="K23" s="7" t="inlineStr">
+        <is>
+          <t>26500</t>
+        </is>
       </c>
       <c r="L23" s="1" t="inlineStr"/>
     </row>
@@ -1139,7 +1151,7 @@
       <c r="B26" s="2" t="inlineStr"/>
       <c r="C26" s="1" t="inlineStr">
         <is>
-          <t>01/Jun/2025</t>
+          <t>2025-06-01 00:00:00</t>
         </is>
       </c>
       <c r="D26" s="1" t="inlineStr">
@@ -1165,8 +1177,10 @@
         </is>
       </c>
       <c r="J26" s="1" t="inlineStr"/>
-      <c r="K26" s="7" t="n">
-        <v>30100</v>
+      <c r="K26" s="7" t="inlineStr">
+        <is>
+          <t>30100</t>
+        </is>
       </c>
       <c r="L26" s="1" t="inlineStr"/>
     </row>
@@ -1219,7 +1233,7 @@
       <c r="B29" s="12" t="inlineStr"/>
       <c r="C29" s="11" t="inlineStr">
         <is>
-          <t>01/Jun/2025</t>
+          <t>2025-06-01 00:00:00</t>
         </is>
       </c>
       <c r="D29" s="11" t="inlineStr">
@@ -1244,8 +1258,10 @@
           <t>27654</t>
         </is>
       </c>
-      <c r="J29" s="15" t="n">
-        <v>9000000</v>
+      <c r="J29" s="15" t="inlineStr">
+        <is>
+          <t>9000000</t>
+        </is>
       </c>
       <c r="K29" s="11" t="inlineStr"/>
       <c r="L29" s="11" t="inlineStr">
@@ -1321,7 +1337,7 @@
       <c r="B32" s="2" t="inlineStr"/>
       <c r="C32" s="1" t="inlineStr">
         <is>
-          <t>01/Jun/2025</t>
+          <t>2025-06-01 00:00:00</t>
         </is>
       </c>
       <c r="D32" s="1" t="inlineStr">
@@ -1346,8 +1362,10 @@
           <t>1357</t>
         </is>
       </c>
-      <c r="J32" s="7" t="n">
-        <v>905515</v>
+      <c r="J32" s="7" t="inlineStr">
+        <is>
+          <t>905515</t>
+        </is>
       </c>
       <c r="K32" s="1" t="inlineStr"/>
       <c r="L32" s="1" t="inlineStr"/>
@@ -1398,7 +1416,7 @@
       <c r="B35" s="2" t="inlineStr"/>
       <c r="C35" s="1" t="inlineStr">
         <is>
-          <t>01/Jun/2025</t>
+          <t>2025-06-01 00:00:00</t>
         </is>
       </c>
       <c r="D35" s="1" t="inlineStr">
@@ -1423,8 +1441,10 @@
           <t>1360</t>
         </is>
       </c>
-      <c r="J35" s="7" t="n">
-        <v>6835265</v>
+      <c r="J35" s="7" t="inlineStr">
+        <is>
+          <t>6835265</t>
+        </is>
       </c>
       <c r="K35" s="1" t="inlineStr"/>
       <c r="L35" s="1" t="inlineStr"/>
@@ -1478,7 +1498,7 @@
       <c r="B38" s="19" t="inlineStr"/>
       <c r="C38" s="18" t="inlineStr">
         <is>
-          <t>02/Jun/2025</t>
+          <t>2025-06-02 00:00:00</t>
         </is>
       </c>
       <c r="D38" s="18" t="inlineStr">
@@ -1503,8 +1523,10 @@
           <t>1364</t>
         </is>
       </c>
-      <c r="J38" s="22" t="n">
-        <v>18027176.54</v>
+      <c r="J38" s="22" t="inlineStr">
+        <is>
+          <t>18027176.54</t>
+        </is>
       </c>
       <c r="K38" s="18" t="inlineStr"/>
       <c r="L38" s="18" t="inlineStr">
@@ -1531,8 +1553,10 @@
       <c r="G39" s="18" t="inlineStr"/>
       <c r="H39" s="18" t="inlineStr"/>
       <c r="I39" s="18" t="inlineStr"/>
-      <c r="J39" s="22" t="n">
-        <v>9706941.220000001</v>
+      <c r="J39" s="22" t="inlineStr">
+        <is>
+          <t>9706941.22</t>
+        </is>
       </c>
       <c r="K39" s="18" t="inlineStr"/>
       <c r="L39" s="18" t="inlineStr">
@@ -1560,8 +1584,10 @@
       <c r="H40" s="18" t="inlineStr"/>
       <c r="I40" s="18" t="inlineStr"/>
       <c r="J40" s="18" t="inlineStr"/>
-      <c r="K40" s="22" t="n">
-        <v>614549.95</v>
+      <c r="K40" s="22" t="inlineStr">
+        <is>
+          <t>614549.95</t>
+        </is>
       </c>
       <c r="L40" s="18" t="inlineStr">
         <is>
@@ -1588,8 +1614,10 @@
       <c r="H41" s="18" t="inlineStr"/>
       <c r="I41" s="18" t="inlineStr"/>
       <c r="J41" s="18" t="inlineStr"/>
-      <c r="K41" s="22" t="n">
-        <v>27119567.81</v>
+      <c r="K41" s="22" t="inlineStr">
+        <is>
+          <t>27119567.81</t>
+        </is>
       </c>
       <c r="L41" s="18" t="inlineStr">
         <is>
@@ -1664,7 +1692,7 @@
       <c r="B44" s="2" t="inlineStr"/>
       <c r="C44" s="1" t="inlineStr">
         <is>
-          <t>03/Jun/2025</t>
+          <t>2025-06-03 00:00:00</t>
         </is>
       </c>
       <c r="D44" s="1" t="inlineStr">
@@ -1690,8 +1718,10 @@
         </is>
       </c>
       <c r="J44" s="1" t="inlineStr"/>
-      <c r="K44" s="7" t="n">
-        <v>22529</v>
+      <c r="K44" s="7" t="inlineStr">
+        <is>
+          <t>22529</t>
+        </is>
       </c>
       <c r="L44" s="1" t="inlineStr"/>
     </row>
@@ -1740,7 +1770,7 @@
       <c r="B47" s="2" t="inlineStr"/>
       <c r="C47" s="1" t="inlineStr">
         <is>
-          <t>03/Jun/2025</t>
+          <t>2025-06-03 00:00:00</t>
         </is>
       </c>
       <c r="D47" s="1" t="inlineStr">
@@ -1766,8 +1796,10 @@
         </is>
       </c>
       <c r="J47" s="1" t="inlineStr"/>
-      <c r="K47" s="7" t="n">
-        <v>8263</v>
+      <c r="K47" s="7" t="inlineStr">
+        <is>
+          <t>8263</t>
+        </is>
       </c>
       <c r="L47" s="1" t="inlineStr"/>
     </row>
@@ -1817,7 +1849,7 @@
       <c r="B50" s="2" t="inlineStr"/>
       <c r="C50" s="1" t="inlineStr">
         <is>
-          <t>03/Jun/2025</t>
+          <t>2025-06-03 00:00:00</t>
         </is>
       </c>
       <c r="D50" s="1" t="inlineStr">
@@ -1843,8 +1875,10 @@
         </is>
       </c>
       <c r="J50" s="1" t="inlineStr"/>
-      <c r="K50" s="7" t="n">
-        <v>10057</v>
+      <c r="K50" s="7" t="inlineStr">
+        <is>
+          <t>10057</t>
+        </is>
       </c>
       <c r="L50" s="1" t="inlineStr"/>
     </row>
@@ -1893,7 +1927,7 @@
       <c r="B53" s="2" t="inlineStr"/>
       <c r="C53" s="1" t="inlineStr">
         <is>
-          <t>03/Jun/2025</t>
+          <t>2025-06-03 00:00:00</t>
         </is>
       </c>
       <c r="D53" s="1" t="inlineStr">
@@ -1919,8 +1953,10 @@
         </is>
       </c>
       <c r="J53" s="1" t="inlineStr"/>
-      <c r="K53" s="7" t="n">
-        <v>36664</v>
+      <c r="K53" s="7" t="inlineStr">
+        <is>
+          <t>36664</t>
+        </is>
       </c>
       <c r="L53" s="1" t="inlineStr"/>
     </row>
@@ -1969,7 +2005,7 @@
       <c r="B56" s="2" t="inlineStr"/>
       <c r="C56" s="1" t="inlineStr">
         <is>
-          <t>03/Jun/2025</t>
+          <t>2025-06-03 00:00:00</t>
         </is>
       </c>
       <c r="D56" s="1" t="inlineStr">
@@ -1995,8 +2031,10 @@
         </is>
       </c>
       <c r="J56" s="1" t="inlineStr"/>
-      <c r="K56" s="7" t="n">
-        <v>11928.4</v>
+      <c r="K56" s="7" t="inlineStr">
+        <is>
+          <t>11928.4</t>
+        </is>
       </c>
       <c r="L56" s="1" t="inlineStr"/>
     </row>
@@ -2045,7 +2083,7 @@
       <c r="B59" s="2" t="inlineStr"/>
       <c r="C59" s="1" t="inlineStr">
         <is>
-          <t>03/Jun/2025</t>
+          <t>2025-06-03 00:00:00</t>
         </is>
       </c>
       <c r="D59" s="1" t="inlineStr">
@@ -2071,8 +2109,10 @@
         </is>
       </c>
       <c r="J59" s="1" t="inlineStr"/>
-      <c r="K59" s="7" t="n">
-        <v>21029</v>
+      <c r="K59" s="7" t="inlineStr">
+        <is>
+          <t>21029</t>
+        </is>
       </c>
       <c r="L59" s="1" t="inlineStr"/>
     </row>
@@ -2121,7 +2161,7 @@
       <c r="B62" s="2" t="inlineStr"/>
       <c r="C62" s="1" t="inlineStr">
         <is>
-          <t>03/Jun/2025</t>
+          <t>2025-06-03 00:00:00</t>
         </is>
       </c>
       <c r="D62" s="1" t="inlineStr">
@@ -2147,8 +2187,10 @@
         </is>
       </c>
       <c r="J62" s="1" t="inlineStr"/>
-      <c r="K62" s="7" t="n">
-        <v>78711</v>
+      <c r="K62" s="7" t="inlineStr">
+        <is>
+          <t>78711</t>
+        </is>
       </c>
       <c r="L62" s="1" t="inlineStr"/>
     </row>
@@ -2197,7 +2239,7 @@
       <c r="B65" s="2" t="inlineStr"/>
       <c r="C65" s="1" t="inlineStr">
         <is>
-          <t>03/Jun/2025</t>
+          <t>2025-06-03 00:00:00</t>
         </is>
       </c>
       <c r="D65" s="1" t="inlineStr">
@@ -2223,8 +2265,10 @@
         </is>
       </c>
       <c r="J65" s="1" t="inlineStr"/>
-      <c r="K65" s="7" t="n">
-        <v>58353</v>
+      <c r="K65" s="7" t="inlineStr">
+        <is>
+          <t>58353</t>
+        </is>
       </c>
       <c r="L65" s="1" t="inlineStr"/>
     </row>
@@ -2273,7 +2317,7 @@
       <c r="B68" s="2" t="inlineStr"/>
       <c r="C68" s="1" t="inlineStr">
         <is>
-          <t>03/Jun/2025</t>
+          <t>2025-06-03 00:00:00</t>
         </is>
       </c>
       <c r="D68" s="1" t="inlineStr">
@@ -2299,8 +2343,10 @@
         </is>
       </c>
       <c r="J68" s="1" t="inlineStr"/>
-      <c r="K68" s="7" t="n">
-        <v>76000</v>
+      <c r="K68" s="7" t="inlineStr">
+        <is>
+          <t>76000</t>
+        </is>
       </c>
       <c r="L68" s="1" t="inlineStr"/>
     </row>
@@ -2350,7 +2396,7 @@
       <c r="B71" s="2" t="inlineStr"/>
       <c r="C71" s="1" t="inlineStr">
         <is>
-          <t>03/Jun/2025</t>
+          <t>2025-06-03 00:00:00</t>
         </is>
       </c>
       <c r="D71" s="1" t="inlineStr">
@@ -2376,8 +2422,10 @@
         </is>
       </c>
       <c r="J71" s="1" t="inlineStr"/>
-      <c r="K71" s="7" t="n">
-        <v>3294.86</v>
+      <c r="K71" s="7" t="inlineStr">
+        <is>
+          <t>3294.86</t>
+        </is>
       </c>
       <c r="L71" s="1" t="inlineStr"/>
     </row>
@@ -2426,7 +2474,7 @@
       <c r="B74" s="2" t="inlineStr"/>
       <c r="C74" s="1" t="inlineStr">
         <is>
-          <t>03/Jun/2025</t>
+          <t>2025-06-03 00:00:00</t>
         </is>
       </c>
       <c r="D74" s="1" t="inlineStr">
@@ -2452,8 +2500,10 @@
         </is>
       </c>
       <c r="J74" s="1" t="inlineStr"/>
-      <c r="K74" s="7" t="n">
-        <v>19489.36</v>
+      <c r="K74" s="7" t="inlineStr">
+        <is>
+          <t>19489.36</t>
+        </is>
       </c>
       <c r="L74" s="1" t="inlineStr"/>
     </row>
@@ -2502,7 +2552,7 @@
       <c r="B77" s="2" t="inlineStr"/>
       <c r="C77" s="1" t="inlineStr">
         <is>
-          <t>03/Jun/2025</t>
+          <t>2025-06-03 00:00:00</t>
         </is>
       </c>
       <c r="D77" s="1" t="inlineStr">
@@ -2528,8 +2578,10 @@
         </is>
       </c>
       <c r="J77" s="1" t="inlineStr"/>
-      <c r="K77" s="7" t="n">
-        <v>11485</v>
+      <c r="K77" s="7" t="inlineStr">
+        <is>
+          <t>11485</t>
+        </is>
       </c>
       <c r="L77" s="1" t="inlineStr"/>
     </row>
@@ -2578,7 +2630,7 @@
       <c r="B80" s="2" t="inlineStr"/>
       <c r="C80" s="1" t="inlineStr">
         <is>
-          <t>03/Jun/2025</t>
+          <t>2025-06-03 00:00:00</t>
         </is>
       </c>
       <c r="D80" s="1" t="inlineStr">
@@ -2604,8 +2656,10 @@
         </is>
       </c>
       <c r="J80" s="1" t="inlineStr"/>
-      <c r="K80" s="7" t="n">
-        <v>27000</v>
+      <c r="K80" s="7" t="inlineStr">
+        <is>
+          <t>27000</t>
+        </is>
       </c>
       <c r="L80" s="1" t="inlineStr"/>
     </row>
@@ -2658,7 +2712,7 @@
       <c r="B83" s="12" t="inlineStr"/>
       <c r="C83" s="11" t="inlineStr">
         <is>
-          <t>03/Jun/2025</t>
+          <t>2025-06-03 00:00:00</t>
         </is>
       </c>
       <c r="D83" s="11" t="inlineStr">
@@ -2684,8 +2738,10 @@
         </is>
       </c>
       <c r="J83" s="11" t="inlineStr"/>
-      <c r="K83" s="15" t="n">
-        <v>600000</v>
+      <c r="K83" s="15" t="inlineStr">
+        <is>
+          <t>600000</t>
+        </is>
       </c>
       <c r="L83" s="11" t="inlineStr">
         <is>
@@ -2764,7 +2820,7 @@
       <c r="B86" s="19" t="inlineStr"/>
       <c r="C86" s="18" t="inlineStr">
         <is>
-          <t>03/Jun/2025</t>
+          <t>2025-06-03 00:00:00</t>
         </is>
       </c>
       <c r="D86" s="18" t="inlineStr">
@@ -2790,8 +2846,10 @@
         </is>
       </c>
       <c r="J86" s="18" t="inlineStr"/>
-      <c r="K86" s="22" t="n">
-        <v>300000</v>
+      <c r="K86" s="22" t="inlineStr">
+        <is>
+          <t>300000</t>
+        </is>
       </c>
       <c r="L86" s="18" t="inlineStr">
         <is>
@@ -2871,7 +2929,7 @@
       <c r="B89" s="12" t="inlineStr"/>
       <c r="C89" s="11" t="inlineStr">
         <is>
-          <t>03/Jun/2025</t>
+          <t>2025-06-03 00:00:00</t>
         </is>
       </c>
       <c r="D89" s="11" t="inlineStr">
@@ -2897,8 +2955,10 @@
         </is>
       </c>
       <c r="J89" s="11" t="inlineStr"/>
-      <c r="K89" s="15" t="n">
-        <v>700000</v>
+      <c r="K89" s="15" t="inlineStr">
+        <is>
+          <t>700000</t>
+        </is>
       </c>
       <c r="L89" s="11" t="inlineStr">
         <is>
@@ -2973,7 +3033,7 @@
       <c r="B92" s="2" t="inlineStr"/>
       <c r="C92" s="1" t="inlineStr">
         <is>
-          <t>03/Jun/2025</t>
+          <t>2025-06-03 00:00:00</t>
         </is>
       </c>
       <c r="D92" s="1" t="inlineStr">
@@ -2999,8 +3059,10 @@
         </is>
       </c>
       <c r="J92" s="1" t="inlineStr"/>
-      <c r="K92" s="7" t="n">
-        <v>225380</v>
+      <c r="K92" s="7" t="inlineStr">
+        <is>
+          <t>225380</t>
+        </is>
       </c>
       <c r="L92" s="1" t="inlineStr"/>
     </row>
@@ -3049,7 +3111,7 @@
       <c r="B95" s="2" t="inlineStr"/>
       <c r="C95" s="1" t="inlineStr">
         <is>
-          <t>03/Jun/2025</t>
+          <t>2025-06-03 00:00:00</t>
         </is>
       </c>
       <c r="D95" s="1" t="inlineStr">
@@ -3075,8 +3137,10 @@
         </is>
       </c>
       <c r="J95" s="1" t="inlineStr"/>
-      <c r="K95" s="7" t="n">
-        <v>50930</v>
+      <c r="K95" s="7" t="inlineStr">
+        <is>
+          <t>50930</t>
+        </is>
       </c>
       <c r="L95" s="1" t="inlineStr"/>
     </row>
@@ -3125,7 +3189,7 @@
       <c r="B98" s="2" t="inlineStr"/>
       <c r="C98" s="1" t="inlineStr">
         <is>
-          <t>03/Jun/2025</t>
+          <t>2025-06-03 00:00:00</t>
         </is>
       </c>
       <c r="D98" s="1" t="inlineStr">
@@ -3151,8 +3215,10 @@
         </is>
       </c>
       <c r="J98" s="1" t="inlineStr"/>
-      <c r="K98" s="7" t="n">
-        <v>256060</v>
+      <c r="K98" s="7" t="inlineStr">
+        <is>
+          <t>256060</t>
+        </is>
       </c>
       <c r="L98" s="1" t="inlineStr"/>
     </row>
@@ -3201,7 +3267,7 @@
       <c r="B101" s="2" t="inlineStr"/>
       <c r="C101" s="1" t="inlineStr">
         <is>
-          <t>03/Jun/2025</t>
+          <t>2025-06-03 00:00:00</t>
         </is>
       </c>
       <c r="D101" s="1" t="inlineStr">
@@ -3227,8 +3293,10 @@
         </is>
       </c>
       <c r="J101" s="1" t="inlineStr"/>
-      <c r="K101" s="7" t="n">
-        <v>10500</v>
+      <c r="K101" s="7" t="inlineStr">
+        <is>
+          <t>10500</t>
+        </is>
       </c>
       <c r="L101" s="1" t="inlineStr"/>
     </row>
@@ -3277,7 +3345,7 @@
       <c r="B104" s="2" t="inlineStr"/>
       <c r="C104" s="1" t="inlineStr">
         <is>
-          <t>03/Jun/2025</t>
+          <t>2025-06-03 00:00:00</t>
         </is>
       </c>
       <c r="D104" s="1" t="inlineStr">
@@ -3303,8 +3371,10 @@
         </is>
       </c>
       <c r="J104" s="1" t="inlineStr"/>
-      <c r="K104" s="7" t="n">
-        <v>22680</v>
+      <c r="K104" s="7" t="inlineStr">
+        <is>
+          <t>22680</t>
+        </is>
       </c>
       <c r="L104" s="1" t="inlineStr"/>
     </row>
@@ -3353,7 +3423,7 @@
       <c r="B107" s="2" t="inlineStr"/>
       <c r="C107" s="1" t="inlineStr">
         <is>
-          <t>03/Jun/2025</t>
+          <t>2025-06-03 00:00:00</t>
         </is>
       </c>
       <c r="D107" s="1" t="inlineStr">
@@ -3379,8 +3449,10 @@
         </is>
       </c>
       <c r="J107" s="1" t="inlineStr"/>
-      <c r="K107" s="7" t="n">
-        <v>11300</v>
+      <c r="K107" s="7" t="inlineStr">
+        <is>
+          <t>11300</t>
+        </is>
       </c>
       <c r="L107" s="1" t="inlineStr"/>
     </row>
@@ -3429,7 +3501,7 @@
       <c r="B110" s="2" t="inlineStr"/>
       <c r="C110" s="1" t="inlineStr">
         <is>
-          <t>03/Jun/2025</t>
+          <t>2025-06-03 00:00:00</t>
         </is>
       </c>
       <c r="D110" s="1" t="inlineStr">
@@ -3455,8 +3527,10 @@
         </is>
       </c>
       <c r="J110" s="1" t="inlineStr"/>
-      <c r="K110" s="7" t="n">
-        <v>230740</v>
+      <c r="K110" s="7" t="inlineStr">
+        <is>
+          <t>230740</t>
+        </is>
       </c>
       <c r="L110" s="1" t="inlineStr"/>
     </row>
@@ -3509,7 +3583,7 @@
       <c r="B113" s="19" t="inlineStr"/>
       <c r="C113" s="18" t="inlineStr">
         <is>
-          <t>03/Jun/2025</t>
+          <t>2025-06-03 00:00:00</t>
         </is>
       </c>
       <c r="D113" s="18" t="inlineStr">
@@ -3535,8 +3609,10 @@
         </is>
       </c>
       <c r="J113" s="18" t="inlineStr"/>
-      <c r="K113" s="22" t="n">
-        <v>100000</v>
+      <c r="K113" s="22" t="inlineStr">
+        <is>
+          <t>100000</t>
+        </is>
       </c>
       <c r="L113" s="18" t="inlineStr">
         <is>
@@ -3611,7 +3687,7 @@
       <c r="B116" s="2" t="inlineStr"/>
       <c r="C116" s="1" t="inlineStr">
         <is>
-          <t>03/Jun/2025</t>
+          <t>2025-06-03 00:00:00</t>
         </is>
       </c>
       <c r="D116" s="1" t="inlineStr">
@@ -3637,8 +3713,10 @@
         </is>
       </c>
       <c r="J116" s="1" t="inlineStr"/>
-      <c r="K116" s="7" t="n">
-        <v>20520</v>
+      <c r="K116" s="7" t="inlineStr">
+        <is>
+          <t>20520</t>
+        </is>
       </c>
       <c r="L116" s="1" t="inlineStr"/>
     </row>
@@ -3687,7 +3765,7 @@
       <c r="B119" s="2" t="inlineStr"/>
       <c r="C119" s="1" t="inlineStr">
         <is>
-          <t>03/Jun/2025</t>
+          <t>2025-06-03 00:00:00</t>
         </is>
       </c>
       <c r="D119" s="1" t="inlineStr">
@@ -3713,8 +3791,10 @@
         </is>
       </c>
       <c r="J119" s="1" t="inlineStr"/>
-      <c r="K119" s="7" t="n">
-        <v>126000</v>
+      <c r="K119" s="7" t="inlineStr">
+        <is>
+          <t>126000</t>
+        </is>
       </c>
       <c r="L119" s="1" t="inlineStr"/>
     </row>
@@ -3763,7 +3843,7 @@
       <c r="B122" s="2" t="inlineStr"/>
       <c r="C122" s="1" t="inlineStr">
         <is>
-          <t>03/Jun/2025</t>
+          <t>2025-06-03 00:00:00</t>
         </is>
       </c>
       <c r="D122" s="1" t="inlineStr">
@@ -3789,8 +3869,10 @@
         </is>
       </c>
       <c r="J122" s="1" t="inlineStr"/>
-      <c r="K122" s="7" t="n">
-        <v>70000</v>
+      <c r="K122" s="7" t="inlineStr">
+        <is>
+          <t>70000</t>
+        </is>
       </c>
       <c r="L122" s="1" t="inlineStr"/>
     </row>
@@ -3839,7 +3921,7 @@
       <c r="B125" s="2" t="inlineStr"/>
       <c r="C125" s="1" t="inlineStr">
         <is>
-          <t>03/Jun/2025</t>
+          <t>2025-06-03 00:00:00</t>
         </is>
       </c>
       <c r="D125" s="1" t="inlineStr">
@@ -3865,8 +3947,10 @@
         </is>
       </c>
       <c r="J125" s="1" t="inlineStr"/>
-      <c r="K125" s="7" t="n">
-        <v>99980</v>
+      <c r="K125" s="7" t="inlineStr">
+        <is>
+          <t>99980</t>
+        </is>
       </c>
       <c r="L125" s="1" t="inlineStr"/>
     </row>
@@ -3915,7 +3999,7 @@
       <c r="B128" s="2" t="inlineStr"/>
       <c r="C128" s="1" t="inlineStr">
         <is>
-          <t>03/Jun/2025</t>
+          <t>2025-06-03 00:00:00</t>
         </is>
       </c>
       <c r="D128" s="1" t="inlineStr">
@@ -3941,8 +4025,10 @@
         </is>
       </c>
       <c r="J128" s="1" t="inlineStr"/>
-      <c r="K128" s="7" t="n">
-        <v>44160</v>
+      <c r="K128" s="7" t="inlineStr">
+        <is>
+          <t>44160</t>
+        </is>
       </c>
       <c r="L128" s="1" t="inlineStr"/>
     </row>
@@ -3991,7 +4077,7 @@
       <c r="B131" s="2" t="inlineStr"/>
       <c r="C131" s="1" t="inlineStr">
         <is>
-          <t>03/Jun/2025</t>
+          <t>2025-06-03 00:00:00</t>
         </is>
       </c>
       <c r="D131" s="1" t="inlineStr">
@@ -4017,8 +4103,10 @@
         </is>
       </c>
       <c r="J131" s="1" t="inlineStr"/>
-      <c r="K131" s="7" t="n">
-        <v>348320</v>
+      <c r="K131" s="7" t="inlineStr">
+        <is>
+          <t>348320</t>
+        </is>
       </c>
       <c r="L131" s="1" t="inlineStr"/>
     </row>
@@ -4067,7 +4155,7 @@
       <c r="B134" s="2" t="inlineStr"/>
       <c r="C134" s="1" t="inlineStr">
         <is>
-          <t>03/Jun/2025</t>
+          <t>2025-06-03 00:00:00</t>
         </is>
       </c>
       <c r="D134" s="1" t="inlineStr">
@@ -4093,8 +4181,10 @@
         </is>
       </c>
       <c r="J134" s="1" t="inlineStr"/>
-      <c r="K134" s="7" t="n">
-        <v>31581.6</v>
+      <c r="K134" s="7" t="inlineStr">
+        <is>
+          <t>31581.6</t>
+        </is>
       </c>
       <c r="L134" s="1" t="inlineStr"/>
     </row>
@@ -4143,7 +4233,7 @@
       <c r="B137" s="2" t="inlineStr"/>
       <c r="C137" s="1" t="inlineStr">
         <is>
-          <t>03/Jun/2025</t>
+          <t>2025-06-03 00:00:00</t>
         </is>
       </c>
       <c r="D137" s="1" t="inlineStr">
@@ -4169,8 +4259,10 @@
         </is>
       </c>
       <c r="J137" s="1" t="inlineStr"/>
-      <c r="K137" s="7" t="n">
-        <v>26100</v>
+      <c r="K137" s="7" t="inlineStr">
+        <is>
+          <t>26100</t>
+        </is>
       </c>
       <c r="L137" s="1" t="inlineStr"/>
     </row>
@@ -4219,7 +4311,7 @@
       <c r="B140" s="2" t="inlineStr"/>
       <c r="C140" s="1" t="inlineStr">
         <is>
-          <t>03/Jun/2025</t>
+          <t>2025-06-03 00:00:00</t>
         </is>
       </c>
       <c r="D140" s="1" t="inlineStr">
@@ -4245,8 +4337,10 @@
         </is>
       </c>
       <c r="J140" s="1" t="inlineStr"/>
-      <c r="K140" s="7" t="n">
-        <v>122265</v>
+      <c r="K140" s="7" t="inlineStr">
+        <is>
+          <t>122265</t>
+        </is>
       </c>
       <c r="L140" s="1" t="inlineStr"/>
     </row>
@@ -4295,7 +4389,7 @@
       <c r="B143" s="2" t="inlineStr"/>
       <c r="C143" s="1" t="inlineStr">
         <is>
-          <t>03/Jun/2025</t>
+          <t>2025-06-03 00:00:00</t>
         </is>
       </c>
       <c r="D143" s="1" t="inlineStr">
@@ -4321,8 +4415,10 @@
         </is>
       </c>
       <c r="J143" s="1" t="inlineStr"/>
-      <c r="K143" s="7" t="n">
-        <v>110920</v>
+      <c r="K143" s="7" t="inlineStr">
+        <is>
+          <t>110920</t>
+        </is>
       </c>
       <c r="L143" s="1" t="inlineStr"/>
     </row>
@@ -4371,7 +4467,7 @@
       <c r="B146" s="2" t="inlineStr"/>
       <c r="C146" s="1" t="inlineStr">
         <is>
-          <t>03/Jun/2025</t>
+          <t>2025-06-03 00:00:00</t>
         </is>
       </c>
       <c r="D146" s="1" t="inlineStr">
@@ -4397,8 +4493,10 @@
         </is>
       </c>
       <c r="J146" s="1" t="inlineStr"/>
-      <c r="K146" s="7" t="n">
-        <v>41400</v>
+      <c r="K146" s="7" t="inlineStr">
+        <is>
+          <t>41400</t>
+        </is>
       </c>
       <c r="L146" s="1" t="inlineStr"/>
     </row>
@@ -4447,7 +4545,7 @@
       <c r="B149" s="2" t="inlineStr"/>
       <c r="C149" s="1" t="inlineStr">
         <is>
-          <t>03/Jun/2025</t>
+          <t>2025-06-03 00:00:00</t>
         </is>
       </c>
       <c r="D149" s="1" t="inlineStr">
@@ -4473,8 +4571,10 @@
         </is>
       </c>
       <c r="J149" s="1" t="inlineStr"/>
-      <c r="K149" s="7" t="n">
-        <v>44676</v>
+      <c r="K149" s="7" t="inlineStr">
+        <is>
+          <t>44676</t>
+        </is>
       </c>
       <c r="L149" s="1" t="inlineStr"/>
     </row>
@@ -4523,7 +4623,7 @@
       <c r="B152" s="2" t="inlineStr"/>
       <c r="C152" s="1" t="inlineStr">
         <is>
-          <t>03/Jun/2025</t>
+          <t>2025-06-03 00:00:00</t>
         </is>
       </c>
       <c r="D152" s="1" t="inlineStr">
@@ -4549,8 +4649,10 @@
         </is>
       </c>
       <c r="J152" s="1" t="inlineStr"/>
-      <c r="K152" s="7" t="n">
-        <v>347445</v>
+      <c r="K152" s="7" t="inlineStr">
+        <is>
+          <t>347445</t>
+        </is>
       </c>
       <c r="L152" s="1" t="inlineStr"/>
     </row>
@@ -4599,7 +4701,7 @@
       <c r="B155" s="2" t="inlineStr"/>
       <c r="C155" s="1" t="inlineStr">
         <is>
-          <t>03/Jun/2025</t>
+          <t>2025-06-03 00:00:00</t>
         </is>
       </c>
       <c r="D155" s="1" t="inlineStr">
@@ -4625,8 +4727,10 @@
         </is>
       </c>
       <c r="J155" s="1" t="inlineStr"/>
-      <c r="K155" s="7" t="n">
-        <v>995220</v>
+      <c r="K155" s="7" t="inlineStr">
+        <is>
+          <t>995220</t>
+        </is>
       </c>
       <c r="L155" s="1" t="inlineStr"/>
     </row>
@@ -4675,7 +4779,7 @@
       <c r="B158" s="2" t="inlineStr"/>
       <c r="C158" s="1" t="inlineStr">
         <is>
-          <t>03/Jun/2025</t>
+          <t>2025-06-03 00:00:00</t>
         </is>
       </c>
       <c r="D158" s="1" t="inlineStr">
@@ -4701,8 +4805,10 @@
         </is>
       </c>
       <c r="J158" s="1" t="inlineStr"/>
-      <c r="K158" s="7" t="n">
-        <v>20880</v>
+      <c r="K158" s="7" t="inlineStr">
+        <is>
+          <t>20880</t>
+        </is>
       </c>
       <c r="L158" s="1" t="inlineStr"/>
     </row>
@@ -4751,7 +4857,7 @@
       <c r="B161" s="2" t="inlineStr"/>
       <c r="C161" s="1" t="inlineStr">
         <is>
-          <t>03/Jun/2025</t>
+          <t>2025-06-03 00:00:00</t>
         </is>
       </c>
       <c r="D161" s="1" t="inlineStr">
@@ -4777,8 +4883,10 @@
         </is>
       </c>
       <c r="J161" s="1" t="inlineStr"/>
-      <c r="K161" s="7" t="n">
-        <v>7200</v>
+      <c r="K161" s="7" t="inlineStr">
+        <is>
+          <t>7200</t>
+        </is>
       </c>
       <c r="L161" s="1" t="inlineStr"/>
     </row>
@@ -4827,7 +4935,7 @@
       <c r="B164" s="2" t="inlineStr"/>
       <c r="C164" s="1" t="inlineStr">
         <is>
-          <t>03/Jun/2025</t>
+          <t>2025-06-03 00:00:00</t>
         </is>
       </c>
       <c r="D164" s="1" t="inlineStr">
@@ -4853,8 +4961,10 @@
         </is>
       </c>
       <c r="J164" s="1" t="inlineStr"/>
-      <c r="K164" s="7" t="n">
-        <v>19800</v>
+      <c r="K164" s="7" t="inlineStr">
+        <is>
+          <t>19800</t>
+        </is>
       </c>
       <c r="L164" s="1" t="inlineStr"/>
     </row>
@@ -4903,7 +5013,7 @@
       <c r="B167" s="2" t="inlineStr"/>
       <c r="C167" s="1" t="inlineStr">
         <is>
-          <t>03/Jun/2025</t>
+          <t>2025-06-03 00:00:00</t>
         </is>
       </c>
       <c r="D167" s="1" t="inlineStr">
@@ -4929,8 +5039,10 @@
         </is>
       </c>
       <c r="J167" s="1" t="inlineStr"/>
-      <c r="K167" s="7" t="n">
-        <v>6120</v>
+      <c r="K167" s="7" t="inlineStr">
+        <is>
+          <t>6120</t>
+        </is>
       </c>
       <c r="L167" s="1" t="inlineStr"/>
     </row>
@@ -4979,7 +5091,7 @@
       <c r="B170" s="2" t="inlineStr"/>
       <c r="C170" s="1" t="inlineStr">
         <is>
-          <t>03/Jun/2025</t>
+          <t>2025-06-03 00:00:00</t>
         </is>
       </c>
       <c r="D170" s="1" t="inlineStr">
@@ -5005,8 +5117,10 @@
         </is>
       </c>
       <c r="J170" s="1" t="inlineStr"/>
-      <c r="K170" s="7" t="n">
-        <v>6240</v>
+      <c r="K170" s="7" t="inlineStr">
+        <is>
+          <t>6240</t>
+        </is>
       </c>
       <c r="L170" s="1" t="inlineStr"/>
     </row>
@@ -5055,7 +5169,7 @@
       <c r="B173" s="2" t="inlineStr"/>
       <c r="C173" s="1" t="inlineStr">
         <is>
-          <t>03/Jun/2025</t>
+          <t>2025-06-03 00:00:00</t>
         </is>
       </c>
       <c r="D173" s="1" t="inlineStr">
@@ -5081,8 +5195,10 @@
         </is>
       </c>
       <c r="J173" s="1" t="inlineStr"/>
-      <c r="K173" s="7" t="n">
-        <v>22000</v>
+      <c r="K173" s="7" t="inlineStr">
+        <is>
+          <t>22000</t>
+        </is>
       </c>
       <c r="L173" s="1" t="inlineStr"/>
     </row>
@@ -5131,7 +5247,7 @@
       <c r="B176" s="2" t="inlineStr"/>
       <c r="C176" s="1" t="inlineStr">
         <is>
-          <t>03/Jun/2025</t>
+          <t>2025-06-03 00:00:00</t>
         </is>
       </c>
       <c r="D176" s="1" t="inlineStr">
@@ -5157,8 +5273,10 @@
         </is>
       </c>
       <c r="J176" s="1" t="inlineStr"/>
-      <c r="K176" s="7" t="n">
-        <v>469812</v>
+      <c r="K176" s="7" t="inlineStr">
+        <is>
+          <t>469812</t>
+        </is>
       </c>
       <c r="L176" s="1" t="inlineStr"/>
     </row>
@@ -5207,7 +5325,7 @@
       <c r="B179" s="2" t="inlineStr"/>
       <c r="C179" s="1" t="inlineStr">
         <is>
-          <t>03/Jun/2025</t>
+          <t>2025-06-03 00:00:00</t>
         </is>
       </c>
       <c r="D179" s="1" t="inlineStr">
@@ -5233,8 +5351,10 @@
         </is>
       </c>
       <c r="J179" s="1" t="inlineStr"/>
-      <c r="K179" s="7" t="n">
-        <v>64000</v>
+      <c r="K179" s="7" t="inlineStr">
+        <is>
+          <t>64000</t>
+        </is>
       </c>
       <c r="L179" s="1" t="inlineStr"/>
     </row>
@@ -5283,7 +5403,7 @@
       <c r="B182" s="2" t="inlineStr"/>
       <c r="C182" s="1" t="inlineStr">
         <is>
-          <t>03/Jun/2025</t>
+          <t>2025-06-03 00:00:00</t>
         </is>
       </c>
       <c r="D182" s="1" t="inlineStr">
@@ -5309,8 +5429,10 @@
         </is>
       </c>
       <c r="J182" s="1" t="inlineStr"/>
-      <c r="K182" s="7" t="n">
-        <v>523260</v>
+      <c r="K182" s="7" t="inlineStr">
+        <is>
+          <t>523260</t>
+        </is>
       </c>
       <c r="L182" s="1" t="inlineStr"/>
     </row>
@@ -5359,7 +5481,7 @@
       <c r="B185" s="2" t="inlineStr"/>
       <c r="C185" s="1" t="inlineStr">
         <is>
-          <t>03/Jun/2025</t>
+          <t>2025-06-03 00:00:00</t>
         </is>
       </c>
       <c r="D185" s="1" t="inlineStr">
@@ -5385,8 +5507,10 @@
         </is>
       </c>
       <c r="J185" s="1" t="inlineStr"/>
-      <c r="K185" s="7" t="n">
-        <v>80325</v>
+      <c r="K185" s="7" t="inlineStr">
+        <is>
+          <t>80325</t>
+        </is>
       </c>
       <c r="L185" s="1" t="inlineStr"/>
     </row>
@@ -5435,7 +5559,7 @@
       <c r="B188" s="2" t="inlineStr"/>
       <c r="C188" s="1" t="inlineStr">
         <is>
-          <t>03/Jun/2025</t>
+          <t>2025-06-03 00:00:00</t>
         </is>
       </c>
       <c r="D188" s="1" t="inlineStr">
@@ -5461,8 +5585,10 @@
         </is>
       </c>
       <c r="J188" s="1" t="inlineStr"/>
-      <c r="K188" s="7" t="n">
-        <v>588395</v>
+      <c r="K188" s="7" t="inlineStr">
+        <is>
+          <t>588395</t>
+        </is>
       </c>
       <c r="L188" s="1" t="inlineStr"/>
     </row>
@@ -5511,7 +5637,7 @@
       <c r="B191" s="2" t="inlineStr"/>
       <c r="C191" s="1" t="inlineStr">
         <is>
-          <t>03/Jun/2025</t>
+          <t>2025-06-03 00:00:00</t>
         </is>
       </c>
       <c r="D191" s="1" t="inlineStr">
@@ -5537,8 +5663,10 @@
         </is>
       </c>
       <c r="J191" s="1" t="inlineStr"/>
-      <c r="K191" s="7" t="n">
-        <v>16600</v>
+      <c r="K191" s="7" t="inlineStr">
+        <is>
+          <t>16600</t>
+        </is>
       </c>
       <c r="L191" s="1" t="inlineStr"/>
     </row>
@@ -5587,7 +5715,7 @@
       <c r="B194" s="2" t="inlineStr"/>
       <c r="C194" s="1" t="inlineStr">
         <is>
-          <t>03/Jun/2025</t>
+          <t>2025-06-03 00:00:00</t>
         </is>
       </c>
       <c r="D194" s="1" t="inlineStr">
@@ -5613,8 +5741,10 @@
         </is>
       </c>
       <c r="J194" s="1" t="inlineStr"/>
-      <c r="K194" s="7" t="n">
-        <v>2200</v>
+      <c r="K194" s="7" t="inlineStr">
+        <is>
+          <t>2200</t>
+        </is>
       </c>
       <c r="L194" s="1" t="inlineStr"/>
     </row>
@@ -5663,7 +5793,7 @@
       <c r="B197" s="2" t="inlineStr"/>
       <c r="C197" s="1" t="inlineStr">
         <is>
-          <t>03/Jun/2025</t>
+          <t>2025-06-03 00:00:00</t>
         </is>
       </c>
       <c r="D197" s="1" t="inlineStr">
@@ -5689,8 +5819,10 @@
         </is>
       </c>
       <c r="J197" s="1" t="inlineStr"/>
-      <c r="K197" s="7" t="n">
-        <v>8400</v>
+      <c r="K197" s="7" t="inlineStr">
+        <is>
+          <t>8400</t>
+        </is>
       </c>
       <c r="L197" s="1" t="inlineStr"/>
     </row>
@@ -5739,7 +5871,7 @@
       <c r="B200" s="2" t="inlineStr"/>
       <c r="C200" s="1" t="inlineStr">
         <is>
-          <t>03/Jun/2025</t>
+          <t>2025-06-03 00:00:00</t>
         </is>
       </c>
       <c r="D200" s="1" t="inlineStr">
@@ -5765,8 +5897,10 @@
         </is>
       </c>
       <c r="J200" s="1" t="inlineStr"/>
-      <c r="K200" s="7" t="n">
-        <v>500000</v>
+      <c r="K200" s="7" t="inlineStr">
+        <is>
+          <t>500000</t>
+        </is>
       </c>
       <c r="L200" s="1" t="inlineStr"/>
     </row>
@@ -5819,7 +5953,7 @@
       <c r="B203" s="12" t="inlineStr"/>
       <c r="C203" s="11" t="inlineStr">
         <is>
-          <t>03/Jun/2025</t>
+          <t>2025-06-03 00:00:00</t>
         </is>
       </c>
       <c r="D203" s="11" t="inlineStr">
@@ -5845,8 +5979,10 @@
         </is>
       </c>
       <c r="J203" s="11" t="inlineStr"/>
-      <c r="K203" s="15" t="n">
-        <v>700000</v>
+      <c r="K203" s="15" t="inlineStr">
+        <is>
+          <t>700000</t>
+        </is>
       </c>
       <c r="L203" s="11" t="inlineStr">
         <is>
@@ -5921,7 +6057,7 @@
       <c r="B206" s="2" t="inlineStr"/>
       <c r="C206" s="1" t="inlineStr">
         <is>
-          <t>03/Jun/2025</t>
+          <t>2025-06-03 00:00:00</t>
         </is>
       </c>
       <c r="D206" s="1" t="inlineStr">
@@ -5947,8 +6083,10 @@
         </is>
       </c>
       <c r="J206" s="1" t="inlineStr"/>
-      <c r="K206" s="7" t="n">
-        <v>200000</v>
+      <c r="K206" s="7" t="inlineStr">
+        <is>
+          <t>200000</t>
+        </is>
       </c>
       <c r="L206" s="1" t="inlineStr"/>
     </row>
@@ -5997,7 +6135,7 @@
       <c r="B209" s="2" t="inlineStr"/>
       <c r="C209" s="1" t="inlineStr">
         <is>
-          <t>03/Jun/2025</t>
+          <t>2025-06-03 00:00:00</t>
         </is>
       </c>
       <c r="D209" s="1" t="inlineStr">
@@ -6023,8 +6161,10 @@
         </is>
       </c>
       <c r="J209" s="1" t="inlineStr"/>
-      <c r="K209" s="7" t="n">
-        <v>19383502.81</v>
+      <c r="K209" s="7" t="inlineStr">
+        <is>
+          <t>19383502.81</t>
+        </is>
       </c>
       <c r="L209" s="1" t="inlineStr"/>
     </row>
@@ -6042,8 +6182,10 @@
       <c r="G210" s="1" t="inlineStr"/>
       <c r="H210" s="1" t="inlineStr"/>
       <c r="I210" s="1" t="inlineStr"/>
-      <c r="J210" s="7" t="n">
-        <v>9524699.43</v>
+      <c r="J210" s="7" t="inlineStr">
+        <is>
+          <t>9524699.43</t>
+        </is>
       </c>
       <c r="K210" s="1" t="inlineStr"/>
       <c r="L210" s="1" t="inlineStr"/>
@@ -6062,8 +6204,10 @@
       <c r="G211" s="1" t="inlineStr"/>
       <c r="H211" s="1" t="inlineStr"/>
       <c r="I211" s="1" t="inlineStr"/>
-      <c r="J211" s="7" t="n">
-        <v>9858803.380000001</v>
+      <c r="J211" s="7" t="inlineStr">
+        <is>
+          <t>9858803.38</t>
+        </is>
       </c>
       <c r="K211" s="1" t="inlineStr"/>
       <c r="L211" s="1" t="inlineStr"/>
@@ -6117,7 +6261,7 @@
       <c r="B214" s="19" t="inlineStr"/>
       <c r="C214" s="18" t="inlineStr">
         <is>
-          <t>04/Jun/2025</t>
+          <t>2025-06-04 00:00:00</t>
         </is>
       </c>
       <c r="D214" s="18" t="inlineStr">
@@ -6143,8 +6287,10 @@
         </is>
       </c>
       <c r="J214" s="18" t="inlineStr"/>
-      <c r="K214" s="22" t="n">
-        <v>200000</v>
+      <c r="K214" s="22" t="inlineStr">
+        <is>
+          <t>200000</t>
+        </is>
       </c>
       <c r="L214" s="18" t="inlineStr">
         <is>
@@ -6223,7 +6369,7 @@
       <c r="B217" s="12" t="inlineStr"/>
       <c r="C217" s="11" t="inlineStr">
         <is>
-          <t>04/Jun/2025</t>
+          <t>2025-06-04 00:00:00</t>
         </is>
       </c>
       <c r="D217" s="11" t="inlineStr">
@@ -6248,8 +6394,10 @@
           <t>1429</t>
         </is>
       </c>
-      <c r="J217" s="15" t="n">
-        <v>41625247.63</v>
+      <c r="J217" s="15" t="inlineStr">
+        <is>
+          <t>41625247.63</t>
+        </is>
       </c>
       <c r="K217" s="11" t="inlineStr"/>
       <c r="L217" s="11" t="inlineStr">
@@ -6276,8 +6424,10 @@
       <c r="G218" s="11" t="inlineStr"/>
       <c r="H218" s="11" t="inlineStr"/>
       <c r="I218" s="11" t="inlineStr"/>
-      <c r="J218" s="15" t="n">
-        <v>54393012.69</v>
+      <c r="J218" s="15" t="inlineStr">
+        <is>
+          <t>54393012.69</t>
+        </is>
       </c>
       <c r="K218" s="11" t="inlineStr"/>
       <c r="L218" s="11" t="inlineStr">
@@ -6304,8 +6454,10 @@
       <c r="G219" s="11" t="inlineStr"/>
       <c r="H219" s="11" t="inlineStr"/>
       <c r="I219" s="11" t="inlineStr"/>
-      <c r="J219" s="15" t="n">
-        <v>784640</v>
+      <c r="J219" s="15" t="inlineStr">
+        <is>
+          <t>784640</t>
+        </is>
       </c>
       <c r="K219" s="11" t="inlineStr"/>
       <c r="L219" s="11" t="inlineStr">
@@ -6333,8 +6485,10 @@
       <c r="H220" s="11" t="inlineStr"/>
       <c r="I220" s="11" t="inlineStr"/>
       <c r="J220" s="11" t="inlineStr"/>
-      <c r="K220" s="15" t="n">
-        <v>43496089</v>
+      <c r="K220" s="15" t="inlineStr">
+        <is>
+          <t>43496089</t>
+        </is>
       </c>
       <c r="L220" s="11" t="inlineStr">
         <is>
@@ -6361,8 +6515,10 @@
       <c r="H221" s="11" t="inlineStr"/>
       <c r="I221" s="11" t="inlineStr"/>
       <c r="J221" s="11" t="inlineStr"/>
-      <c r="K221" s="15" t="n">
-        <v>1302969.4</v>
+      <c r="K221" s="15" t="inlineStr">
+        <is>
+          <t>1302969.4</t>
+        </is>
       </c>
       <c r="L221" s="11" t="inlineStr">
         <is>
@@ -6389,8 +6545,10 @@
       <c r="H222" s="11" t="inlineStr"/>
       <c r="I222" s="11" t="inlineStr"/>
       <c r="J222" s="11" t="inlineStr"/>
-      <c r="K222" s="15" t="n">
-        <v>52003841.92</v>
+      <c r="K222" s="15" t="inlineStr">
+        <is>
+          <t>52003841.92</t>
+        </is>
       </c>
       <c r="L222" s="11" t="inlineStr">
         <is>
@@ -6469,7 +6627,7 @@
       <c r="B225" s="19" t="inlineStr"/>
       <c r="C225" s="18" t="inlineStr">
         <is>
-          <t>04/Jun/2025</t>
+          <t>2025-06-04 00:00:00</t>
         </is>
       </c>
       <c r="D225" s="18" t="inlineStr">
@@ -6495,8 +6653,10 @@
         </is>
       </c>
       <c r="J225" s="18" t="inlineStr"/>
-      <c r="K225" s="22" t="n">
-        <v>36600000</v>
+      <c r="K225" s="22" t="inlineStr">
+        <is>
+          <t>36600000</t>
+        </is>
       </c>
       <c r="L225" s="18" t="inlineStr">
         <is>
@@ -6575,7 +6735,7 @@
       <c r="B228" s="12" t="inlineStr"/>
       <c r="C228" s="11" t="inlineStr">
         <is>
-          <t>05/Jun/2025</t>
+          <t>2025-06-05 00:00:00</t>
         </is>
       </c>
       <c r="D228" s="11" t="inlineStr">
@@ -6601,8 +6761,10 @@
         </is>
       </c>
       <c r="J228" s="11" t="inlineStr"/>
-      <c r="K228" s="15" t="n">
-        <v>62525</v>
+      <c r="K228" s="15" t="inlineStr">
+        <is>
+          <t>62525</t>
+        </is>
       </c>
       <c r="L228" s="11" t="inlineStr">
         <is>
@@ -6677,7 +6839,7 @@
       <c r="B231" s="2" t="inlineStr"/>
       <c r="C231" s="1" t="inlineStr">
         <is>
-          <t>05/Jun/2025</t>
+          <t>2025-06-05 00:00:00</t>
         </is>
       </c>
       <c r="D231" s="1" t="inlineStr">
@@ -6703,8 +6865,10 @@
         </is>
       </c>
       <c r="J231" s="1" t="inlineStr"/>
-      <c r="K231" s="7" t="n">
-        <v>20000</v>
+      <c r="K231" s="7" t="inlineStr">
+        <is>
+          <t>20000</t>
+        </is>
       </c>
       <c r="L231" s="1" t="inlineStr"/>
     </row>
@@ -6753,7 +6917,7 @@
       <c r="B234" s="2" t="inlineStr"/>
       <c r="C234" s="1" t="inlineStr">
         <is>
-          <t>05/Jun/2025</t>
+          <t>2025-06-05 00:00:00</t>
         </is>
       </c>
       <c r="D234" s="1" t="inlineStr">
@@ -6779,8 +6943,10 @@
         </is>
       </c>
       <c r="J234" s="1" t="inlineStr"/>
-      <c r="K234" s="7" t="n">
-        <v>17500</v>
+      <c r="K234" s="7" t="inlineStr">
+        <is>
+          <t>17500</t>
+        </is>
       </c>
       <c r="L234" s="1" t="inlineStr"/>
     </row>
@@ -6829,7 +6995,7 @@
       <c r="B237" s="2" t="inlineStr"/>
       <c r="C237" s="1" t="inlineStr">
         <is>
-          <t>05/Jun/2025</t>
+          <t>2025-06-05 00:00:00</t>
         </is>
       </c>
       <c r="D237" s="1" t="inlineStr">
@@ -6855,8 +7021,10 @@
         </is>
       </c>
       <c r="J237" s="1" t="inlineStr"/>
-      <c r="K237" s="7" t="n">
-        <v>110839</v>
+      <c r="K237" s="7" t="inlineStr">
+        <is>
+          <t>110839</t>
+        </is>
       </c>
       <c r="L237" s="1" t="inlineStr"/>
     </row>
@@ -6909,7 +7077,7 @@
       <c r="B240" s="19" t="inlineStr"/>
       <c r="C240" s="18" t="inlineStr">
         <is>
-          <t>05/Jun/2025</t>
+          <t>2025-06-05 00:00:00</t>
         </is>
       </c>
       <c r="D240" s="18" t="inlineStr">
@@ -6935,8 +7103,10 @@
         </is>
       </c>
       <c r="J240" s="18" t="inlineStr"/>
-      <c r="K240" s="22" t="n">
-        <v>587020</v>
+      <c r="K240" s="22" t="inlineStr">
+        <is>
+          <t>587020</t>
+        </is>
       </c>
       <c r="L240" s="18" t="inlineStr">
         <is>
@@ -7015,7 +7185,7 @@
       <c r="B243" s="12" t="inlineStr"/>
       <c r="C243" s="11" t="inlineStr">
         <is>
-          <t>05/Jun/2025</t>
+          <t>2025-06-05 00:00:00</t>
         </is>
       </c>
       <c r="D243" s="11" t="inlineStr">
@@ -7041,8 +7211,10 @@
         </is>
       </c>
       <c r="J243" s="11" t="inlineStr"/>
-      <c r="K243" s="15" t="n">
-        <v>2250</v>
+      <c r="K243" s="15" t="inlineStr">
+        <is>
+          <t>2250</t>
+        </is>
       </c>
       <c r="L243" s="11" t="inlineStr">
         <is>
@@ -7121,7 +7293,7 @@
       <c r="B246" s="19" t="inlineStr"/>
       <c r="C246" s="18" t="inlineStr">
         <is>
-          <t>05/Jun/2025</t>
+          <t>2025-06-05 00:00:00</t>
         </is>
       </c>
       <c r="D246" s="18" t="inlineStr">
@@ -7147,8 +7319,10 @@
         </is>
       </c>
       <c r="J246" s="18" t="inlineStr"/>
-      <c r="K246" s="22" t="n">
-        <v>62460</v>
+      <c r="K246" s="22" t="inlineStr">
+        <is>
+          <t>62460</t>
+        </is>
       </c>
       <c r="L246" s="18" t="inlineStr">
         <is>
@@ -7227,7 +7401,7 @@
       <c r="B249" s="12" t="inlineStr"/>
       <c r="C249" s="11" t="inlineStr">
         <is>
-          <t>05/Jun/2025</t>
+          <t>2025-06-05 00:00:00</t>
         </is>
       </c>
       <c r="D249" s="11" t="inlineStr">
@@ -7253,8 +7427,10 @@
         </is>
       </c>
       <c r="J249" s="11" t="inlineStr"/>
-      <c r="K249" s="15" t="n">
-        <v>740488</v>
+      <c r="K249" s="15" t="inlineStr">
+        <is>
+          <t>740488</t>
+        </is>
       </c>
       <c r="L249" s="11" t="inlineStr">
         <is>
@@ -7333,7 +7509,7 @@
       <c r="B252" s="19" t="inlineStr"/>
       <c r="C252" s="18" t="inlineStr">
         <is>
-          <t>05/Jun/2025</t>
+          <t>2025-06-05 00:00:00</t>
         </is>
       </c>
       <c r="D252" s="18" t="inlineStr">
@@ -7359,8 +7535,10 @@
         </is>
       </c>
       <c r="J252" s="18" t="inlineStr"/>
-      <c r="K252" s="22" t="n">
-        <v>202621.73</v>
+      <c r="K252" s="22" t="inlineStr">
+        <is>
+          <t>202621.73</t>
+        </is>
       </c>
       <c r="L252" s="18" t="inlineStr">
         <is>
@@ -7439,7 +7617,7 @@
       <c r="B255" s="12" t="inlineStr"/>
       <c r="C255" s="11" t="inlineStr">
         <is>
-          <t>05/Jun/2025</t>
+          <t>2025-06-05 00:00:00</t>
         </is>
       </c>
       <c r="D255" s="11" t="inlineStr">
@@ -7465,8 +7643,10 @@
         </is>
       </c>
       <c r="J255" s="11" t="inlineStr"/>
-      <c r="K255" s="15" t="n">
-        <v>42300</v>
+      <c r="K255" s="15" t="inlineStr">
+        <is>
+          <t>42300</t>
+        </is>
       </c>
       <c r="L255" s="11" t="inlineStr">
         <is>
@@ -7545,7 +7725,7 @@
       <c r="B258" s="19" t="inlineStr"/>
       <c r="C258" s="18" t="inlineStr">
         <is>
-          <t>05/Jun/2025</t>
+          <t>2025-06-05 00:00:00</t>
         </is>
       </c>
       <c r="D258" s="18" t="inlineStr">
@@ -7571,8 +7751,10 @@
         </is>
       </c>
       <c r="J258" s="18" t="inlineStr"/>
-      <c r="K258" s="22" t="n">
-        <v>40500</v>
+      <c r="K258" s="22" t="inlineStr">
+        <is>
+          <t>40500</t>
+        </is>
       </c>
       <c r="L258" s="18" t="inlineStr">
         <is>
@@ -7651,7 +7833,7 @@
       <c r="B261" s="12" t="inlineStr"/>
       <c r="C261" s="11" t="inlineStr">
         <is>
-          <t>05/Jun/2025</t>
+          <t>2025-06-05 00:00:00</t>
         </is>
       </c>
       <c r="D261" s="11" t="inlineStr">
@@ -7677,8 +7859,10 @@
         </is>
       </c>
       <c r="J261" s="11" t="inlineStr"/>
-      <c r="K261" s="15" t="n">
-        <v>511750</v>
+      <c r="K261" s="15" t="inlineStr">
+        <is>
+          <t>511750</t>
+        </is>
       </c>
       <c r="L261" s="11" t="inlineStr">
         <is>
@@ -7757,7 +7941,7 @@
       <c r="B264" s="19" t="inlineStr"/>
       <c r="C264" s="18" t="inlineStr">
         <is>
-          <t>05/Jun/2025</t>
+          <t>2025-06-05 00:00:00</t>
         </is>
       </c>
       <c r="D264" s="18" t="inlineStr">
@@ -7783,8 +7967,10 @@
         </is>
       </c>
       <c r="J264" s="18" t="inlineStr"/>
-      <c r="K264" s="22" t="n">
-        <v>669595</v>
+      <c r="K264" s="22" t="inlineStr">
+        <is>
+          <t>669595</t>
+        </is>
       </c>
       <c r="L264" s="18" t="inlineStr">
         <is>
@@ -7863,7 +8049,7 @@
       <c r="B267" s="12" t="inlineStr"/>
       <c r="C267" s="11" t="inlineStr">
         <is>
-          <t>05/Jun/2025</t>
+          <t>2025-06-05 00:00:00</t>
         </is>
       </c>
       <c r="D267" s="11" t="inlineStr">
@@ -7889,8 +8075,10 @@
         </is>
       </c>
       <c r="J267" s="11" t="inlineStr"/>
-      <c r="K267" s="15" t="n">
-        <v>66980</v>
+      <c r="K267" s="15" t="inlineStr">
+        <is>
+          <t>66980</t>
+        </is>
       </c>
       <c r="L267" s="11" t="inlineStr">
         <is>
@@ -7969,7 +8157,7 @@
       <c r="B270" s="19" t="inlineStr"/>
       <c r="C270" s="18" t="inlineStr">
         <is>
-          <t>05/Jun/2025</t>
+          <t>2025-06-05 00:00:00</t>
         </is>
       </c>
       <c r="D270" s="18" t="inlineStr">
@@ -7995,8 +8183,10 @@
         </is>
       </c>
       <c r="J270" s="18" t="inlineStr"/>
-      <c r="K270" s="22" t="n">
-        <v>12300</v>
+      <c r="K270" s="22" t="inlineStr">
+        <is>
+          <t>12300</t>
+        </is>
       </c>
       <c r="L270" s="18" t="inlineStr">
         <is>
@@ -8075,7 +8265,7 @@
       <c r="B273" s="12" t="inlineStr"/>
       <c r="C273" s="11" t="inlineStr">
         <is>
-          <t>05/Jun/2025</t>
+          <t>2025-06-05 00:00:00</t>
         </is>
       </c>
       <c r="D273" s="11" t="inlineStr">
@@ -8101,8 +8291,10 @@
         </is>
       </c>
       <c r="J273" s="11" t="inlineStr"/>
-      <c r="K273" s="15" t="n">
-        <v>590</v>
+      <c r="K273" s="15" t="inlineStr">
+        <is>
+          <t>590</t>
+        </is>
       </c>
       <c r="L273" s="11" t="inlineStr">
         <is>
@@ -8181,7 +8373,7 @@
       <c r="B276" s="19" t="inlineStr"/>
       <c r="C276" s="18" t="inlineStr">
         <is>
-          <t>05/Jun/2025</t>
+          <t>2025-06-05 00:00:00</t>
         </is>
       </c>
       <c r="D276" s="18" t="inlineStr">
@@ -8207,8 +8399,10 @@
         </is>
       </c>
       <c r="J276" s="18" t="inlineStr"/>
-      <c r="K276" s="22" t="n">
-        <v>9000</v>
+      <c r="K276" s="22" t="inlineStr">
+        <is>
+          <t>9000</t>
+        </is>
       </c>
       <c r="L276" s="18" t="inlineStr">
         <is>
@@ -8287,7 +8481,7 @@
       <c r="B279" s="12" t="inlineStr"/>
       <c r="C279" s="11" t="inlineStr">
         <is>
-          <t>05/Jun/2025</t>
+          <t>2025-06-05 00:00:00</t>
         </is>
       </c>
       <c r="D279" s="11" t="inlineStr">
@@ -8313,8 +8507,10 @@
         </is>
       </c>
       <c r="J279" s="11" t="inlineStr"/>
-      <c r="K279" s="15" t="n">
-        <v>9600</v>
+      <c r="K279" s="15" t="inlineStr">
+        <is>
+          <t>9600</t>
+        </is>
       </c>
       <c r="L279" s="11" t="inlineStr">
         <is>
@@ -8393,7 +8589,7 @@
       <c r="B282" s="19" t="inlineStr"/>
       <c r="C282" s="18" t="inlineStr">
         <is>
-          <t>05/Jun/2025</t>
+          <t>2025-06-05 00:00:00</t>
         </is>
       </c>
       <c r="D282" s="18" t="inlineStr">
@@ -8419,8 +8615,10 @@
         </is>
       </c>
       <c r="J282" s="18" t="inlineStr"/>
-      <c r="K282" s="22" t="n">
-        <v>128327</v>
+      <c r="K282" s="22" t="inlineStr">
+        <is>
+          <t>128327</t>
+        </is>
       </c>
       <c r="L282" s="18" t="inlineStr">
         <is>
@@ -8499,7 +8697,7 @@
       <c r="B285" s="12" t="inlineStr"/>
       <c r="C285" s="11" t="inlineStr">
         <is>
-          <t>05/Jun/2025</t>
+          <t>2025-06-05 00:00:00</t>
         </is>
       </c>
       <c r="D285" s="11" t="inlineStr">
@@ -8525,8 +8723,10 @@
         </is>
       </c>
       <c r="J285" s="11" t="inlineStr"/>
-      <c r="K285" s="15" t="n">
-        <v>131125</v>
+      <c r="K285" s="15" t="inlineStr">
+        <is>
+          <t>131125</t>
+        </is>
       </c>
       <c r="L285" s="11" t="inlineStr">
         <is>
@@ -8605,7 +8805,7 @@
       <c r="B288" s="19" t="inlineStr"/>
       <c r="C288" s="18" t="inlineStr">
         <is>
-          <t>05/Jun/2025</t>
+          <t>2025-06-05 00:00:00</t>
         </is>
       </c>
       <c r="D288" s="18" t="inlineStr">
@@ -8631,8 +8831,10 @@
         </is>
       </c>
       <c r="J288" s="18" t="inlineStr"/>
-      <c r="K288" s="22" t="n">
-        <v>63065</v>
+      <c r="K288" s="22" t="inlineStr">
+        <is>
+          <t>63065</t>
+        </is>
       </c>
       <c r="L288" s="18" t="inlineStr">
         <is>
@@ -8711,7 +8913,7 @@
       <c r="B291" s="12" t="inlineStr"/>
       <c r="C291" s="11" t="inlineStr">
         <is>
-          <t>05/Jun/2025</t>
+          <t>2025-06-05 00:00:00</t>
         </is>
       </c>
       <c r="D291" s="11" t="inlineStr">
@@ -8737,8 +8939,10 @@
         </is>
       </c>
       <c r="J291" s="11" t="inlineStr"/>
-      <c r="K291" s="15" t="n">
-        <v>230000</v>
+      <c r="K291" s="15" t="inlineStr">
+        <is>
+          <t>230000</t>
+        </is>
       </c>
       <c r="L291" s="11" t="inlineStr">
         <is>
@@ -8817,7 +9021,7 @@
       <c r="B294" s="19" t="inlineStr"/>
       <c r="C294" s="18" t="inlineStr">
         <is>
-          <t>05/Jun/2025</t>
+          <t>2025-06-05 00:00:00</t>
         </is>
       </c>
       <c r="D294" s="18" t="inlineStr">
@@ -8843,8 +9047,10 @@
         </is>
       </c>
       <c r="J294" s="18" t="inlineStr"/>
-      <c r="K294" s="22" t="n">
-        <v>293250</v>
+      <c r="K294" s="22" t="inlineStr">
+        <is>
+          <t>293250</t>
+        </is>
       </c>
       <c r="L294" s="18" t="inlineStr">
         <is>
@@ -8923,7 +9129,7 @@
       <c r="B297" s="12" t="inlineStr"/>
       <c r="C297" s="11" t="inlineStr">
         <is>
-          <t>05/Jun/2025</t>
+          <t>2025-06-05 00:00:00</t>
         </is>
       </c>
       <c r="D297" s="11" t="inlineStr">
@@ -8949,8 +9155,10 @@
         </is>
       </c>
       <c r="J297" s="11" t="inlineStr"/>
-      <c r="K297" s="15" t="n">
-        <v>6750</v>
+      <c r="K297" s="15" t="inlineStr">
+        <is>
+          <t>6750</t>
+        </is>
       </c>
       <c r="L297" s="11" t="inlineStr">
         <is>
@@ -9029,7 +9237,7 @@
       <c r="B300" s="19" t="inlineStr"/>
       <c r="C300" s="18" t="inlineStr">
         <is>
-          <t>05/Jun/2025</t>
+          <t>2025-06-05 00:00:00</t>
         </is>
       </c>
       <c r="D300" s="18" t="inlineStr">
@@ -9055,8 +9263,10 @@
         </is>
       </c>
       <c r="J300" s="18" t="inlineStr"/>
-      <c r="K300" s="22" t="n">
-        <v>496219</v>
+      <c r="K300" s="22" t="inlineStr">
+        <is>
+          <t>496219</t>
+        </is>
       </c>
       <c r="L300" s="18" t="inlineStr">
         <is>
@@ -9135,7 +9345,7 @@
       <c r="B303" s="12" t="inlineStr"/>
       <c r="C303" s="11" t="inlineStr">
         <is>
-          <t>05/Jun/2025</t>
+          <t>2025-06-05 00:00:00</t>
         </is>
       </c>
       <c r="D303" s="11" t="inlineStr">
@@ -9161,8 +9371,10 @@
         </is>
       </c>
       <c r="J303" s="11" t="inlineStr"/>
-      <c r="K303" s="15" t="n">
-        <v>56500</v>
+      <c r="K303" s="15" t="inlineStr">
+        <is>
+          <t>56500</t>
+        </is>
       </c>
       <c r="L303" s="11" t="inlineStr">
         <is>
@@ -9241,7 +9453,7 @@
       <c r="B306" s="19" t="inlineStr"/>
       <c r="C306" s="18" t="inlineStr">
         <is>
-          <t>05/Jun/2025</t>
+          <t>2025-06-05 00:00:00</t>
         </is>
       </c>
       <c r="D306" s="18" t="inlineStr">
@@ -9267,8 +9479,10 @@
         </is>
       </c>
       <c r="J306" s="18" t="inlineStr"/>
-      <c r="K306" s="22" t="n">
-        <v>195820</v>
+      <c r="K306" s="22" t="inlineStr">
+        <is>
+          <t>195820</t>
+        </is>
       </c>
       <c r="L306" s="18" t="inlineStr">
         <is>
@@ -9347,7 +9561,7 @@
       <c r="B309" s="12" t="inlineStr"/>
       <c r="C309" s="11" t="inlineStr">
         <is>
-          <t>05/Jun/2025</t>
+          <t>2025-06-05 00:00:00</t>
         </is>
       </c>
       <c r="D309" s="11" t="inlineStr">
@@ -9373,8 +9587,10 @@
         </is>
       </c>
       <c r="J309" s="11" t="inlineStr"/>
-      <c r="K309" s="15" t="n">
-        <v>15300</v>
+      <c r="K309" s="15" t="inlineStr">
+        <is>
+          <t>15300</t>
+        </is>
       </c>
       <c r="L309" s="11" t="inlineStr">
         <is>
@@ -9453,7 +9669,7 @@
       <c r="B312" s="19" t="inlineStr"/>
       <c r="C312" s="18" t="inlineStr">
         <is>
-          <t>05/Jun/2025</t>
+          <t>2025-06-05 00:00:00</t>
         </is>
       </c>
       <c r="D312" s="18" t="inlineStr">
@@ -9479,8 +9695,10 @@
         </is>
       </c>
       <c r="J312" s="18" t="inlineStr"/>
-      <c r="K312" s="22" t="n">
-        <v>96000</v>
+      <c r="K312" s="22" t="inlineStr">
+        <is>
+          <t>96000</t>
+        </is>
       </c>
       <c r="L312" s="18" t="inlineStr">
         <is>
@@ -9559,7 +9777,7 @@
       <c r="B315" s="12" t="inlineStr"/>
       <c r="C315" s="11" t="inlineStr">
         <is>
-          <t>05/Jun/2025</t>
+          <t>2025-06-05 00:00:00</t>
         </is>
       </c>
       <c r="D315" s="11" t="inlineStr">
@@ -9585,8 +9803,10 @@
         </is>
       </c>
       <c r="J315" s="11" t="inlineStr"/>
-      <c r="K315" s="15" t="n">
-        <v>10562.5</v>
+      <c r="K315" s="15" t="inlineStr">
+        <is>
+          <t>10562.5</t>
+        </is>
       </c>
       <c r="L315" s="11" t="inlineStr">
         <is>
@@ -9665,7 +9885,7 @@
       <c r="B318" s="19" t="inlineStr"/>
       <c r="C318" s="18" t="inlineStr">
         <is>
-          <t>05/Jun/2025</t>
+          <t>2025-06-05 00:00:00</t>
         </is>
       </c>
       <c r="D318" s="18" t="inlineStr">
@@ -9691,8 +9911,10 @@
         </is>
       </c>
       <c r="J318" s="18" t="inlineStr"/>
-      <c r="K318" s="22" t="n">
-        <v>2700</v>
+      <c r="K318" s="22" t="inlineStr">
+        <is>
+          <t>2700</t>
+        </is>
       </c>
       <c r="L318" s="18" t="inlineStr">
         <is>
@@ -9771,7 +9993,7 @@
       <c r="B321" s="12" t="inlineStr"/>
       <c r="C321" s="11" t="inlineStr">
         <is>
-          <t>05/Jun/2025</t>
+          <t>2025-06-05 00:00:00</t>
         </is>
       </c>
       <c r="D321" s="11" t="inlineStr">
@@ -9797,8 +10019,10 @@
         </is>
       </c>
       <c r="J321" s="11" t="inlineStr"/>
-      <c r="K321" s="15" t="n">
-        <v>26291.76</v>
+      <c r="K321" s="15" t="inlineStr">
+        <is>
+          <t>26291.76</t>
+        </is>
       </c>
       <c r="L321" s="11" t="inlineStr">
         <is>
@@ -9877,7 +10101,7 @@
       <c r="B324" s="19" t="inlineStr"/>
       <c r="C324" s="18" t="inlineStr">
         <is>
-          <t>05/Jun/2025</t>
+          <t>2025-06-05 00:00:00</t>
         </is>
       </c>
       <c r="D324" s="18" t="inlineStr">
@@ -9903,8 +10127,10 @@
         </is>
       </c>
       <c r="J324" s="18" t="inlineStr"/>
-      <c r="K324" s="22" t="n">
-        <v>129240</v>
+      <c r="K324" s="22" t="inlineStr">
+        <is>
+          <t>129240</t>
+        </is>
       </c>
       <c r="L324" s="18" t="inlineStr">
         <is>
@@ -9983,7 +10209,7 @@
       <c r="B327" s="12" t="inlineStr"/>
       <c r="C327" s="11" t="inlineStr">
         <is>
-          <t>05/Jun/2025</t>
+          <t>2025-06-05 00:00:00</t>
         </is>
       </c>
       <c r="D327" s="11" t="inlineStr">
@@ -10009,8 +10235,10 @@
         </is>
       </c>
       <c r="J327" s="11" t="inlineStr"/>
-      <c r="K327" s="15" t="n">
-        <v>15044</v>
+      <c r="K327" s="15" t="inlineStr">
+        <is>
+          <t>15044</t>
+        </is>
       </c>
       <c r="L327" s="11" t="inlineStr">
         <is>
@@ -10089,7 +10317,7 @@
       <c r="B330" s="19" t="inlineStr"/>
       <c r="C330" s="18" t="inlineStr">
         <is>
-          <t>05/Jun/2025</t>
+          <t>2025-06-05 00:00:00</t>
         </is>
       </c>
       <c r="D330" s="18" t="inlineStr">
@@ -10115,8 +10343,10 @@
         </is>
       </c>
       <c r="J330" s="18" t="inlineStr"/>
-      <c r="K330" s="22" t="n">
-        <v>4967.7</v>
+      <c r="K330" s="22" t="inlineStr">
+        <is>
+          <t>4967.7</t>
+        </is>
       </c>
       <c r="L330" s="18" t="inlineStr">
         <is>
@@ -10195,7 +10425,7 @@
       <c r="B333" s="12" t="inlineStr"/>
       <c r="C333" s="11" t="inlineStr">
         <is>
-          <t>05/Jun/2025</t>
+          <t>2025-06-05 00:00:00</t>
         </is>
       </c>
       <c r="D333" s="11" t="inlineStr">
@@ -10221,8 +10451,10 @@
         </is>
       </c>
       <c r="J333" s="11" t="inlineStr"/>
-      <c r="K333" s="15" t="n">
-        <v>8697.92</v>
+      <c r="K333" s="15" t="inlineStr">
+        <is>
+          <t>8697.92</t>
+        </is>
       </c>
       <c r="L333" s="11" t="inlineStr">
         <is>
@@ -10301,7 +10533,7 @@
       <c r="B336" s="19" t="inlineStr"/>
       <c r="C336" s="18" t="inlineStr">
         <is>
-          <t>05/Jun/2025</t>
+          <t>2025-06-05 00:00:00</t>
         </is>
       </c>
       <c r="D336" s="18" t="inlineStr">
@@ -10327,8 +10559,10 @@
         </is>
       </c>
       <c r="J336" s="18" t="inlineStr"/>
-      <c r="K336" s="22" t="n">
-        <v>15000</v>
+      <c r="K336" s="22" t="inlineStr">
+        <is>
+          <t>15000</t>
+        </is>
       </c>
       <c r="L336" s="18" t="inlineStr">
         <is>
@@ -10407,7 +10641,7 @@
       <c r="B339" s="12" t="inlineStr"/>
       <c r="C339" s="11" t="inlineStr">
         <is>
-          <t>05/Jun/2025</t>
+          <t>2025-06-05 00:00:00</t>
         </is>
       </c>
       <c r="D339" s="11" t="inlineStr">
@@ -10433,8 +10667,10 @@
         </is>
       </c>
       <c r="J339" s="11" t="inlineStr"/>
-      <c r="K339" s="15" t="n">
-        <v>235248</v>
+      <c r="K339" s="15" t="inlineStr">
+        <is>
+          <t>235248</t>
+        </is>
       </c>
       <c r="L339" s="11" t="inlineStr">
         <is>
@@ -10513,7 +10749,7 @@
       <c r="B342" s="19" t="inlineStr"/>
       <c r="C342" s="18" t="inlineStr">
         <is>
-          <t>05/Jun/2025</t>
+          <t>2025-06-05 00:00:00</t>
         </is>
       </c>
       <c r="D342" s="18" t="inlineStr">
@@ -10539,8 +10775,10 @@
         </is>
       </c>
       <c r="J342" s="18" t="inlineStr"/>
-      <c r="K342" s="22" t="n">
-        <v>197500</v>
+      <c r="K342" s="22" t="inlineStr">
+        <is>
+          <t>197500</t>
+        </is>
       </c>
       <c r="L342" s="18" t="inlineStr">
         <is>
@@ -10619,7 +10857,7 @@
       <c r="B345" s="12" t="inlineStr"/>
       <c r="C345" s="11" t="inlineStr">
         <is>
-          <t>05/Jun/2025</t>
+          <t>2025-06-05 00:00:00</t>
         </is>
       </c>
       <c r="D345" s="11" t="inlineStr">
@@ -10645,8 +10883,10 @@
         </is>
       </c>
       <c r="J345" s="11" t="inlineStr"/>
-      <c r="K345" s="15" t="n">
-        <v>14000</v>
+      <c r="K345" s="15" t="inlineStr">
+        <is>
+          <t>14000</t>
+        </is>
       </c>
       <c r="L345" s="11" t="inlineStr">
         <is>
@@ -10725,7 +10965,7 @@
       <c r="B348" s="19" t="inlineStr"/>
       <c r="C348" s="18" t="inlineStr">
         <is>
-          <t>05/Jun/2025</t>
+          <t>2025-06-05 00:00:00</t>
         </is>
       </c>
       <c r="D348" s="18" t="inlineStr">
@@ -10751,8 +10991,10 @@
         </is>
       </c>
       <c r="J348" s="18" t="inlineStr"/>
-      <c r="K348" s="22" t="n">
-        <v>121231</v>
+      <c r="K348" s="22" t="inlineStr">
+        <is>
+          <t>121231</t>
+        </is>
       </c>
       <c r="L348" s="18" t="inlineStr">
         <is>
@@ -10831,7 +11073,7 @@
       <c r="B351" s="12" t="inlineStr"/>
       <c r="C351" s="11" t="inlineStr">
         <is>
-          <t>05/Jun/2025</t>
+          <t>2025-06-05 00:00:00</t>
         </is>
       </c>
       <c r="D351" s="11" t="inlineStr">
@@ -10857,8 +11099,10 @@
         </is>
       </c>
       <c r="J351" s="11" t="inlineStr"/>
-      <c r="K351" s="15" t="n">
-        <v>63811</v>
+      <c r="K351" s="15" t="inlineStr">
+        <is>
+          <t>63811</t>
+        </is>
       </c>
       <c r="L351" s="11" t="inlineStr">
         <is>
@@ -10937,7 +11181,7 @@
       <c r="B354" s="19" t="inlineStr"/>
       <c r="C354" s="18" t="inlineStr">
         <is>
-          <t>05/Jun/2025</t>
+          <t>2025-06-05 00:00:00</t>
         </is>
       </c>
       <c r="D354" s="18" t="inlineStr">
@@ -10963,8 +11207,10 @@
         </is>
       </c>
       <c r="J354" s="18" t="inlineStr"/>
-      <c r="K354" s="22" t="n">
-        <v>2844</v>
+      <c r="K354" s="22" t="inlineStr">
+        <is>
+          <t>2844</t>
+        </is>
       </c>
       <c r="L354" s="18" t="inlineStr">
         <is>
@@ -11043,7 +11289,7 @@
       <c r="B357" s="12" t="inlineStr"/>
       <c r="C357" s="11" t="inlineStr">
         <is>
-          <t>05/Jun/2025</t>
+          <t>2025-06-05 00:00:00</t>
         </is>
       </c>
       <c r="D357" s="11" t="inlineStr">
@@ -11069,8 +11315,10 @@
         </is>
       </c>
       <c r="J357" s="11" t="inlineStr"/>
-      <c r="K357" s="15" t="n">
-        <v>10173</v>
+      <c r="K357" s="15" t="inlineStr">
+        <is>
+          <t>10173</t>
+        </is>
       </c>
       <c r="L357" s="11" t="inlineStr">
         <is>
@@ -11149,7 +11397,7 @@
       <c r="B360" s="19" t="inlineStr"/>
       <c r="C360" s="18" t="inlineStr">
         <is>
-          <t>15/Jun/2025</t>
+          <t>2025-06-15 00:00:00</t>
         </is>
       </c>
       <c r="D360" s="18" t="inlineStr">
@@ -11175,8 +11423,10 @@
         </is>
       </c>
       <c r="J360" s="18" t="inlineStr"/>
-      <c r="K360" s="22" t="n">
-        <v>1725</v>
+      <c r="K360" s="22" t="inlineStr">
+        <is>
+          <t>1725</t>
+        </is>
       </c>
       <c r="L360" s="18" t="inlineStr">
         <is>
@@ -11255,7 +11505,7 @@
       <c r="B363" s="12" t="inlineStr"/>
       <c r="C363" s="11" t="inlineStr">
         <is>
-          <t>16/Jun/2025</t>
+          <t>2025-06-16 00:00:00</t>
         </is>
       </c>
       <c r="D363" s="11" t="inlineStr">
@@ -11281,8 +11531,10 @@
         </is>
       </c>
       <c r="J363" s="11" t="inlineStr"/>
-      <c r="K363" s="15" t="n">
-        <v>1725</v>
+      <c r="K363" s="15" t="inlineStr">
+        <is>
+          <t>1725</t>
+        </is>
       </c>
       <c r="L363" s="11" t="inlineStr">
         <is>
@@ -11361,7 +11613,7 @@
       <c r="B366" s="19" t="inlineStr"/>
       <c r="C366" s="18" t="inlineStr">
         <is>
-          <t>17/Jun/2025</t>
+          <t>2025-06-17 00:00:00</t>
         </is>
       </c>
       <c r="D366" s="18" t="inlineStr">
@@ -11387,8 +11639,10 @@
         </is>
       </c>
       <c r="J366" s="18" t="inlineStr"/>
-      <c r="K366" s="22" t="n">
-        <v>3172250</v>
+      <c r="K366" s="22" t="inlineStr">
+        <is>
+          <t>3172250</t>
+        </is>
       </c>
       <c r="L366" s="18" t="inlineStr">
         <is>
@@ -11463,7 +11717,7 @@
       <c r="B369" s="2" t="inlineStr"/>
       <c r="C369" s="1" t="inlineStr">
         <is>
-          <t>18/Jun/2025</t>
+          <t>2025-06-18 00:00:00</t>
         </is>
       </c>
       <c r="D369" s="1" t="inlineStr">
@@ -11489,8 +11743,10 @@
         </is>
       </c>
       <c r="J369" s="1" t="inlineStr"/>
-      <c r="K369" s="7" t="n">
-        <v>88042</v>
+      <c r="K369" s="7" t="inlineStr">
+        <is>
+          <t>88042</t>
+        </is>
       </c>
       <c r="L369" s="1" t="inlineStr"/>
     </row>
@@ -11539,7 +11795,7 @@
       <c r="B372" s="2" t="inlineStr"/>
       <c r="C372" s="1" t="inlineStr">
         <is>
-          <t>18/Jun/2025</t>
+          <t>2025-06-18 00:00:00</t>
         </is>
       </c>
       <c r="D372" s="1" t="inlineStr">
@@ -11565,8 +11821,10 @@
         </is>
       </c>
       <c r="J372" s="1" t="inlineStr"/>
-      <c r="K372" s="7" t="n">
-        <v>226590</v>
+      <c r="K372" s="7" t="inlineStr">
+        <is>
+          <t>226590</t>
+        </is>
       </c>
       <c r="L372" s="1" t="inlineStr"/>
     </row>
@@ -11619,7 +11877,7 @@
       <c r="B375" s="12" t="inlineStr"/>
       <c r="C375" s="11" t="inlineStr">
         <is>
-          <t>21/Jun/2025</t>
+          <t>2025-06-21 00:00:00</t>
         </is>
       </c>
       <c r="D375" s="11" t="inlineStr">
@@ -11645,8 +11903,10 @@
         </is>
       </c>
       <c r="J375" s="11" t="inlineStr"/>
-      <c r="K375" s="15" t="n">
-        <v>200000</v>
+      <c r="K375" s="15" t="inlineStr">
+        <is>
+          <t>200000</t>
+        </is>
       </c>
       <c r="L375" s="11" t="inlineStr">
         <is>
@@ -11725,7 +11985,7 @@
       <c r="B378" s="19" t="inlineStr"/>
       <c r="C378" s="18" t="inlineStr">
         <is>
-          <t>23/Jun/2025</t>
+          <t>2025-06-23 00:00:00</t>
         </is>
       </c>
       <c r="D378" s="18" t="inlineStr">
@@ -11751,8 +12011,10 @@
         </is>
       </c>
       <c r="J378" s="18" t="inlineStr"/>
-      <c r="K378" s="22" t="n">
-        <v>62067.7</v>
+      <c r="K378" s="22" t="inlineStr">
+        <is>
+          <t>62067.7</t>
+        </is>
       </c>
       <c r="L378" s="18" t="inlineStr">
         <is>
@@ -11831,7 +12093,7 @@
       <c r="B381" s="12" t="inlineStr"/>
       <c r="C381" s="11" t="inlineStr">
         <is>
-          <t>23/Jun/2025</t>
+          <t>2025-06-23 00:00:00</t>
         </is>
       </c>
       <c r="D381" s="11" t="inlineStr">
@@ -11857,8 +12119,10 @@
         </is>
       </c>
       <c r="J381" s="11" t="inlineStr"/>
-      <c r="K381" s="15" t="n">
-        <v>359367.81</v>
+      <c r="K381" s="15" t="inlineStr">
+        <is>
+          <t>359367.81</t>
+        </is>
       </c>
       <c r="L381" s="11" t="inlineStr">
         <is>
@@ -11937,7 +12201,7 @@
       <c r="B384" s="19" t="inlineStr"/>
       <c r="C384" s="18" t="inlineStr">
         <is>
-          <t>23/Jun/2025</t>
+          <t>2025-06-23 00:00:00</t>
         </is>
       </c>
       <c r="D384" s="18" t="inlineStr">
@@ -11963,8 +12227,10 @@
         </is>
       </c>
       <c r="J384" s="18" t="inlineStr"/>
-      <c r="K384" s="22" t="n">
-        <v>7127.53</v>
+      <c r="K384" s="22" t="inlineStr">
+        <is>
+          <t>7127.53</t>
+        </is>
       </c>
       <c r="L384" s="18" t="inlineStr">
         <is>
@@ -12043,7 +12309,7 @@
       <c r="B387" s="12" t="inlineStr"/>
       <c r="C387" s="11" t="inlineStr">
         <is>
-          <t>23/Jun/2025</t>
+          <t>2025-06-23 00:00:00</t>
         </is>
       </c>
       <c r="D387" s="11" t="inlineStr">
@@ -12069,8 +12335,10 @@
         </is>
       </c>
       <c r="J387" s="11" t="inlineStr"/>
-      <c r="K387" s="15" t="n">
-        <v>33701.29</v>
+      <c r="K387" s="15" t="inlineStr">
+        <is>
+          <t>33701.29</t>
+        </is>
       </c>
       <c r="L387" s="11" t="inlineStr">
         <is>
@@ -12145,7 +12413,7 @@
       <c r="B390" s="2" t="inlineStr"/>
       <c r="C390" s="1" t="inlineStr">
         <is>
-          <t>23/Jun/2025</t>
+          <t>2025-06-23 00:00:00</t>
         </is>
       </c>
       <c r="D390" s="1" t="inlineStr">
@@ -12171,8 +12439,10 @@
         </is>
       </c>
       <c r="J390" s="1" t="inlineStr"/>
-      <c r="K390" s="7" t="n">
-        <v>24000000</v>
+      <c r="K390" s="7" t="inlineStr">
+        <is>
+          <t>24000000</t>
+        </is>
       </c>
       <c r="L390" s="1" t="inlineStr"/>
     </row>
@@ -12225,7 +12495,7 @@
       <c r="B393" s="19" t="inlineStr"/>
       <c r="C393" s="18" t="inlineStr">
         <is>
-          <t>24/Jun/2025</t>
+          <t>2025-06-24 00:00:00</t>
         </is>
       </c>
       <c r="D393" s="18" t="inlineStr">
@@ -12251,8 +12521,10 @@
         </is>
       </c>
       <c r="J393" s="18" t="inlineStr"/>
-      <c r="K393" s="22" t="n">
-        <v>1235000</v>
+      <c r="K393" s="22" t="inlineStr">
+        <is>
+          <t>1235000</t>
+        </is>
       </c>
       <c r="L393" s="18" t="inlineStr">
         <is>
@@ -12327,7 +12599,7 @@
       <c r="B396" s="2" t="inlineStr"/>
       <c r="C396" s="1" t="inlineStr">
         <is>
-          <t>25/Jun/2025</t>
+          <t>2025-06-25 00:00:00</t>
         </is>
       </c>
       <c r="D396" s="1" t="inlineStr">
@@ -12353,8 +12625,10 @@
         </is>
       </c>
       <c r="J396" s="1" t="inlineStr"/>
-      <c r="K396" s="7" t="n">
-        <v>1300000</v>
+      <c r="K396" s="7" t="inlineStr">
+        <is>
+          <t>1300000</t>
+        </is>
       </c>
       <c r="L396" s="1" t="inlineStr"/>
     </row>
@@ -12407,7 +12681,7 @@
       <c r="B399" s="12" t="inlineStr"/>
       <c r="C399" s="11" t="inlineStr">
         <is>
-          <t>26/Jun/2025</t>
+          <t>2025-06-26 00:00:00</t>
         </is>
       </c>
       <c r="D399" s="11" t="inlineStr">
@@ -12433,8 +12707,10 @@
         </is>
       </c>
       <c r="J399" s="11" t="inlineStr"/>
-      <c r="K399" s="15" t="n">
-        <v>43496089</v>
+      <c r="K399" s="15" t="inlineStr">
+        <is>
+          <t>43496089</t>
+        </is>
       </c>
       <c r="L399" s="11" t="inlineStr">
         <is>
@@ -12513,7 +12789,7 @@
       <c r="B402" s="19" t="inlineStr"/>
       <c r="C402" s="18" t="inlineStr">
         <is>
-          <t>30/Jun/2025</t>
+          <t>2025-06-30 00:00:00</t>
         </is>
       </c>
       <c r="D402" s="18" t="inlineStr">
@@ -12538,8 +12814,10 @@
           <t>1515</t>
         </is>
       </c>
-      <c r="J402" s="22" t="n">
-        <v>20733</v>
+      <c r="J402" s="22" t="inlineStr">
+        <is>
+          <t>20733</t>
+        </is>
       </c>
       <c r="K402" s="18" t="inlineStr"/>
       <c r="L402" s="18" t="inlineStr">
@@ -12566,8 +12844,10 @@
       <c r="G403" s="18" t="inlineStr"/>
       <c r="H403" s="18" t="inlineStr"/>
       <c r="I403" s="18" t="inlineStr"/>
-      <c r="J403" s="22" t="n">
-        <v>201597</v>
+      <c r="J403" s="22" t="inlineStr">
+        <is>
+          <t>201597</t>
+        </is>
       </c>
       <c r="K403" s="18" t="inlineStr"/>
       <c r="L403" s="18" t="inlineStr">
@@ -12594,8 +12874,10 @@
       <c r="G404" s="18" t="inlineStr"/>
       <c r="H404" s="18" t="inlineStr"/>
       <c r="I404" s="18" t="inlineStr"/>
-      <c r="J404" s="22" t="n">
-        <v>254538</v>
+      <c r="J404" s="22" t="inlineStr">
+        <is>
+          <t>254538</t>
+        </is>
       </c>
       <c r="K404" s="18" t="inlineStr"/>
       <c r="L404" s="18" t="inlineStr">
@@ -12622,8 +12904,10 @@
       <c r="G405" s="18" t="inlineStr"/>
       <c r="H405" s="18" t="inlineStr"/>
       <c r="I405" s="18" t="inlineStr"/>
-      <c r="J405" s="22" t="n">
-        <v>33990</v>
+      <c r="J405" s="22" t="inlineStr">
+        <is>
+          <t>33990</t>
+        </is>
       </c>
       <c r="K405" s="18" t="inlineStr"/>
       <c r="L405" s="18" t="inlineStr">
@@ -12650,8 +12934,10 @@
       <c r="G406" s="18" t="inlineStr"/>
       <c r="H406" s="18" t="inlineStr"/>
       <c r="I406" s="18" t="inlineStr"/>
-      <c r="J406" s="22" t="n">
-        <v>858619</v>
+      <c r="J406" s="22" t="inlineStr">
+        <is>
+          <t>858619</t>
+        </is>
       </c>
       <c r="K406" s="18" t="inlineStr"/>
       <c r="L406" s="18" t="inlineStr">
@@ -12678,8 +12964,10 @@
       <c r="G407" s="18" t="inlineStr"/>
       <c r="H407" s="18" t="inlineStr"/>
       <c r="I407" s="18" t="inlineStr"/>
-      <c r="J407" s="22" t="n">
-        <v>76763</v>
+      <c r="J407" s="22" t="inlineStr">
+        <is>
+          <t>76763</t>
+        </is>
       </c>
       <c r="K407" s="18" t="inlineStr"/>
       <c r="L407" s="18" t="inlineStr">
@@ -12706,8 +12994,10 @@
       <c r="G408" s="18" t="inlineStr"/>
       <c r="H408" s="18" t="inlineStr"/>
       <c r="I408" s="18" t="inlineStr"/>
-      <c r="J408" s="22" t="n">
-        <v>127689</v>
+      <c r="J408" s="22" t="inlineStr">
+        <is>
+          <t>127689</t>
+        </is>
       </c>
       <c r="K408" s="18" t="inlineStr"/>
       <c r="L408" s="18" t="inlineStr">
@@ -12734,8 +13024,10 @@
       <c r="G409" s="18" t="inlineStr"/>
       <c r="H409" s="18" t="inlineStr"/>
       <c r="I409" s="18" t="inlineStr"/>
-      <c r="J409" s="22" t="n">
-        <v>283417</v>
+      <c r="J409" s="22" t="inlineStr">
+        <is>
+          <t>283417</t>
+        </is>
       </c>
       <c r="K409" s="18" t="inlineStr"/>
       <c r="L409" s="18" t="inlineStr">
@@ -12762,8 +13054,10 @@
       <c r="G410" s="18" t="inlineStr"/>
       <c r="H410" s="18" t="inlineStr"/>
       <c r="I410" s="18" t="inlineStr"/>
-      <c r="J410" s="22" t="n">
-        <v>484192</v>
+      <c r="J410" s="22" t="inlineStr">
+        <is>
+          <t>484192</t>
+        </is>
       </c>
       <c r="K410" s="18" t="inlineStr"/>
       <c r="L410" s="18" t="inlineStr">
@@ -12790,8 +13084,10 @@
       <c r="G411" s="18" t="inlineStr"/>
       <c r="H411" s="18" t="inlineStr"/>
       <c r="I411" s="18" t="inlineStr"/>
-      <c r="J411" s="22" t="n">
-        <v>80266</v>
+      <c r="J411" s="22" t="inlineStr">
+        <is>
+          <t>80266</t>
+        </is>
       </c>
       <c r="K411" s="18" t="inlineStr"/>
       <c r="L411" s="18" t="inlineStr">
@@ -12818,8 +13114,10 @@
       <c r="G412" s="18" t="inlineStr"/>
       <c r="H412" s="18" t="inlineStr"/>
       <c r="I412" s="18" t="inlineStr"/>
-      <c r="J412" s="22" t="n">
-        <v>84844</v>
+      <c r="J412" s="22" t="inlineStr">
+        <is>
+          <t>84844</t>
+        </is>
       </c>
       <c r="K412" s="18" t="inlineStr"/>
       <c r="L412" s="18" t="inlineStr">
@@ -12846,8 +13144,10 @@
       <c r="G413" s="18" t="inlineStr"/>
       <c r="H413" s="18" t="inlineStr"/>
       <c r="I413" s="18" t="inlineStr"/>
-      <c r="J413" s="22" t="n">
-        <v>127326</v>
+      <c r="J413" s="22" t="inlineStr">
+        <is>
+          <t>127326</t>
+        </is>
       </c>
       <c r="K413" s="18" t="inlineStr"/>
       <c r="L413" s="18" t="inlineStr">
@@ -12874,8 +13174,10 @@
       <c r="G414" s="18" t="inlineStr"/>
       <c r="H414" s="18" t="inlineStr"/>
       <c r="I414" s="18" t="inlineStr"/>
-      <c r="J414" s="22" t="n">
-        <v>376537</v>
+      <c r="J414" s="22" t="inlineStr">
+        <is>
+          <t>376537</t>
+        </is>
       </c>
       <c r="K414" s="18" t="inlineStr"/>
       <c r="L414" s="18" t="inlineStr">
@@ -12902,8 +13204,10 @@
       <c r="G415" s="18" t="inlineStr"/>
       <c r="H415" s="18" t="inlineStr"/>
       <c r="I415" s="18" t="inlineStr"/>
-      <c r="J415" s="22" t="n">
-        <v>123502</v>
+      <c r="J415" s="22" t="inlineStr">
+        <is>
+          <t>123502</t>
+        </is>
       </c>
       <c r="K415" s="18" t="inlineStr"/>
       <c r="L415" s="18" t="inlineStr">
@@ -12930,8 +13234,10 @@
       <c r="G416" s="18" t="inlineStr"/>
       <c r="H416" s="18" t="inlineStr"/>
       <c r="I416" s="18" t="inlineStr"/>
-      <c r="J416" s="22" t="n">
-        <v>148561</v>
+      <c r="J416" s="22" t="inlineStr">
+        <is>
+          <t>148561</t>
+        </is>
       </c>
       <c r="K416" s="18" t="inlineStr"/>
       <c r="L416" s="18" t="inlineStr">
@@ -12958,8 +13264,10 @@
       <c r="G417" s="18" t="inlineStr"/>
       <c r="H417" s="18" t="inlineStr"/>
       <c r="I417" s="18" t="inlineStr"/>
-      <c r="J417" s="22" t="n">
-        <v>14523</v>
+      <c r="J417" s="22" t="inlineStr">
+        <is>
+          <t>14523</t>
+        </is>
       </c>
       <c r="K417" s="18" t="inlineStr"/>
       <c r="L417" s="18" t="inlineStr">
@@ -12986,8 +13294,10 @@
       <c r="G418" s="18" t="inlineStr"/>
       <c r="H418" s="18" t="inlineStr"/>
       <c r="I418" s="18" t="inlineStr"/>
-      <c r="J418" s="22" t="n">
-        <v>42740</v>
+      <c r="J418" s="22" t="inlineStr">
+        <is>
+          <t>42740</t>
+        </is>
       </c>
       <c r="K418" s="18" t="inlineStr"/>
       <c r="L418" s="18" t="inlineStr">
@@ -13014,8 +13324,10 @@
       <c r="G419" s="18" t="inlineStr"/>
       <c r="H419" s="18" t="inlineStr"/>
       <c r="I419" s="18" t="inlineStr"/>
-      <c r="J419" s="22" t="n">
-        <v>97269</v>
+      <c r="J419" s="22" t="inlineStr">
+        <is>
+          <t>97269</t>
+        </is>
       </c>
       <c r="K419" s="18" t="inlineStr"/>
       <c r="L419" s="18" t="inlineStr">
@@ -13042,8 +13354,10 @@
       <c r="G420" s="18" t="inlineStr"/>
       <c r="H420" s="18" t="inlineStr"/>
       <c r="I420" s="18" t="inlineStr"/>
-      <c r="J420" s="22" t="n">
-        <v>236926</v>
+      <c r="J420" s="22" t="inlineStr">
+        <is>
+          <t>236926</t>
+        </is>
       </c>
       <c r="K420" s="18" t="inlineStr"/>
       <c r="L420" s="18" t="inlineStr">
@@ -13070,8 +13384,10 @@
       <c r="G421" s="18" t="inlineStr"/>
       <c r="H421" s="18" t="inlineStr"/>
       <c r="I421" s="18" t="inlineStr"/>
-      <c r="J421" s="22" t="n">
-        <v>1650</v>
+      <c r="J421" s="22" t="inlineStr">
+        <is>
+          <t>1650</t>
+        </is>
       </c>
       <c r="K421" s="18" t="inlineStr"/>
       <c r="L421" s="18" t="inlineStr">
@@ -13098,8 +13414,10 @@
       <c r="G422" s="18" t="inlineStr"/>
       <c r="H422" s="18" t="inlineStr"/>
       <c r="I422" s="18" t="inlineStr"/>
-      <c r="J422" s="22" t="n">
-        <v>6384</v>
+      <c r="J422" s="22" t="inlineStr">
+        <is>
+          <t>6384</t>
+        </is>
       </c>
       <c r="K422" s="18" t="inlineStr"/>
       <c r="L422" s="18" t="inlineStr">
@@ -13126,8 +13444,10 @@
       <c r="G423" s="18" t="inlineStr"/>
       <c r="H423" s="18" t="inlineStr"/>
       <c r="I423" s="18" t="inlineStr"/>
-      <c r="J423" s="22" t="n">
-        <v>31163</v>
+      <c r="J423" s="22" t="inlineStr">
+        <is>
+          <t>31163</t>
+        </is>
       </c>
       <c r="K423" s="18" t="inlineStr"/>
       <c r="L423" s="18" t="inlineStr">
@@ -13154,8 +13474,10 @@
       <c r="G424" s="18" t="inlineStr"/>
       <c r="H424" s="18" t="inlineStr"/>
       <c r="I424" s="18" t="inlineStr"/>
-      <c r="J424" s="22" t="n">
-        <v>3838</v>
+      <c r="J424" s="22" t="inlineStr">
+        <is>
+          <t>3838</t>
+        </is>
       </c>
       <c r="K424" s="18" t="inlineStr"/>
       <c r="L424" s="18" t="inlineStr">
@@ -13182,8 +13504,10 @@
       <c r="G425" s="18" t="inlineStr"/>
       <c r="H425" s="18" t="inlineStr"/>
       <c r="I425" s="18" t="inlineStr"/>
-      <c r="J425" s="22" t="n">
-        <v>8138</v>
+      <c r="J425" s="22" t="inlineStr">
+        <is>
+          <t>8138</t>
+        </is>
       </c>
       <c r="K425" s="18" t="inlineStr"/>
       <c r="L425" s="18" t="inlineStr">
@@ -13210,8 +13534,10 @@
       <c r="G426" s="18" t="inlineStr"/>
       <c r="H426" s="18" t="inlineStr"/>
       <c r="I426" s="18" t="inlineStr"/>
-      <c r="J426" s="22" t="n">
-        <v>1302</v>
+      <c r="J426" s="22" t="inlineStr">
+        <is>
+          <t>1302</t>
+        </is>
       </c>
       <c r="K426" s="18" t="inlineStr"/>
       <c r="L426" s="18" t="inlineStr">
@@ -13238,8 +13564,10 @@
       <c r="G427" s="18" t="inlineStr"/>
       <c r="H427" s="18" t="inlineStr"/>
       <c r="I427" s="18" t="inlineStr"/>
-      <c r="J427" s="22" t="n">
-        <v>4570</v>
+      <c r="J427" s="22" t="inlineStr">
+        <is>
+          <t>4570</t>
+        </is>
       </c>
       <c r="K427" s="18" t="inlineStr"/>
       <c r="L427" s="18" t="inlineStr">
@@ -13266,8 +13594,10 @@
       <c r="G428" s="18" t="inlineStr"/>
       <c r="H428" s="18" t="inlineStr"/>
       <c r="I428" s="18" t="inlineStr"/>
-      <c r="J428" s="22" t="n">
-        <v>3853</v>
+      <c r="J428" s="22" t="inlineStr">
+        <is>
+          <t>3853</t>
+        </is>
       </c>
       <c r="K428" s="18" t="inlineStr"/>
       <c r="L428" s="18" t="inlineStr">
@@ -13294,8 +13624,10 @@
       <c r="G429" s="18" t="inlineStr"/>
       <c r="H429" s="18" t="inlineStr"/>
       <c r="I429" s="18" t="inlineStr"/>
-      <c r="J429" s="22" t="n">
-        <v>12953</v>
+      <c r="J429" s="22" t="inlineStr">
+        <is>
+          <t>12953</t>
+        </is>
       </c>
       <c r="K429" s="18" t="inlineStr"/>
       <c r="L429" s="18" t="inlineStr">
@@ -13322,8 +13654,10 @@
       <c r="G430" s="18" t="inlineStr"/>
       <c r="H430" s="18" t="inlineStr"/>
       <c r="I430" s="18" t="inlineStr"/>
-      <c r="J430" s="22" t="n">
-        <v>6933</v>
+      <c r="J430" s="22" t="inlineStr">
+        <is>
+          <t>6933</t>
+        </is>
       </c>
       <c r="K430" s="18" t="inlineStr"/>
       <c r="L430" s="18" t="inlineStr">
@@ -13350,8 +13684,10 @@
       <c r="G431" s="18" t="inlineStr"/>
       <c r="H431" s="18" t="inlineStr"/>
       <c r="I431" s="18" t="inlineStr"/>
-      <c r="J431" s="22" t="n">
-        <v>3133</v>
+      <c r="J431" s="22" t="inlineStr">
+        <is>
+          <t>3133</t>
+        </is>
       </c>
       <c r="K431" s="18" t="inlineStr"/>
       <c r="L431" s="18" t="inlineStr">
@@ -13378,8 +13714,10 @@
       <c r="G432" s="18" t="inlineStr"/>
       <c r="H432" s="18" t="inlineStr"/>
       <c r="I432" s="18" t="inlineStr"/>
-      <c r="J432" s="22" t="n">
-        <v>2153</v>
+      <c r="J432" s="22" t="inlineStr">
+        <is>
+          <t>2153</t>
+        </is>
       </c>
       <c r="K432" s="18" t="inlineStr"/>
       <c r="L432" s="18" t="inlineStr">
@@ -13406,8 +13744,10 @@
       <c r="G433" s="18" t="inlineStr"/>
       <c r="H433" s="18" t="inlineStr"/>
       <c r="I433" s="18" t="inlineStr"/>
-      <c r="J433" s="22" t="n">
-        <v>2605</v>
+      <c r="J433" s="22" t="inlineStr">
+        <is>
+          <t>2605</t>
+        </is>
       </c>
       <c r="K433" s="18" t="inlineStr"/>
       <c r="L433" s="18" t="inlineStr">
@@ -13434,8 +13774,10 @@
       <c r="G434" s="18" t="inlineStr"/>
       <c r="H434" s="18" t="inlineStr"/>
       <c r="I434" s="18" t="inlineStr"/>
-      <c r="J434" s="22" t="n">
-        <v>14165</v>
+      <c r="J434" s="22" t="inlineStr">
+        <is>
+          <t>14165</t>
+        </is>
       </c>
       <c r="K434" s="18" t="inlineStr"/>
       <c r="L434" s="18" t="inlineStr">
@@ -13462,8 +13804,10 @@
       <c r="G435" s="18" t="inlineStr"/>
       <c r="H435" s="18" t="inlineStr"/>
       <c r="I435" s="18" t="inlineStr"/>
-      <c r="J435" s="22" t="n">
-        <v>1700</v>
+      <c r="J435" s="22" t="inlineStr">
+        <is>
+          <t>1700</t>
+        </is>
       </c>
       <c r="K435" s="18" t="inlineStr"/>
       <c r="L435" s="18" t="inlineStr">
@@ -13491,8 +13835,10 @@
       <c r="H436" s="18" t="inlineStr"/>
       <c r="I436" s="18" t="inlineStr"/>
       <c r="J436" s="18" t="inlineStr"/>
-      <c r="K436" s="22" t="n">
-        <v>140181</v>
+      <c r="K436" s="22" t="inlineStr">
+        <is>
+          <t>140181</t>
+        </is>
       </c>
       <c r="L436" s="18" t="inlineStr">
         <is>
@@ -13519,8 +13865,10 @@
       <c r="H437" s="18" t="inlineStr"/>
       <c r="I437" s="18" t="inlineStr"/>
       <c r="J437" s="18" t="inlineStr"/>
-      <c r="K437" s="22" t="n">
-        <v>2741</v>
+      <c r="K437" s="22" t="inlineStr">
+        <is>
+          <t>2741</t>
+        </is>
       </c>
       <c r="L437" s="18" t="inlineStr">
         <is>
@@ -13547,8 +13895,10 @@
       <c r="H438" s="18" t="inlineStr"/>
       <c r="I438" s="18" t="inlineStr"/>
       <c r="J438" s="18" t="inlineStr"/>
-      <c r="K438" s="22" t="n">
-        <v>250</v>
+      <c r="K438" s="22" t="inlineStr">
+        <is>
+          <t>250</t>
+        </is>
       </c>
       <c r="L438" s="18" t="inlineStr">
         <is>
@@ -13575,8 +13925,10 @@
       <c r="H439" s="18" t="inlineStr"/>
       <c r="I439" s="18" t="inlineStr"/>
       <c r="J439" s="18" t="inlineStr"/>
-      <c r="K439" s="22" t="n">
-        <v>10692</v>
+      <c r="K439" s="22" t="inlineStr">
+        <is>
+          <t>10692</t>
+        </is>
       </c>
       <c r="L439" s="18" t="inlineStr">
         <is>
@@ -13603,8 +13955,10 @@
       <c r="H440" s="18" t="inlineStr"/>
       <c r="I440" s="18" t="inlineStr"/>
       <c r="J440" s="18" t="inlineStr"/>
-      <c r="K440" s="22" t="n">
-        <v>272</v>
+      <c r="K440" s="22" t="inlineStr">
+        <is>
+          <t>272</t>
+        </is>
       </c>
       <c r="L440" s="18" t="inlineStr">
         <is>
@@ -13631,8 +13985,10 @@
       <c r="H441" s="18" t="inlineStr"/>
       <c r="I441" s="18" t="inlineStr"/>
       <c r="J441" s="18" t="inlineStr"/>
-      <c r="K441" s="22" t="n">
-        <v>2620</v>
+      <c r="K441" s="22" t="inlineStr">
+        <is>
+          <t>2620</t>
+        </is>
       </c>
       <c r="L441" s="18" t="inlineStr">
         <is>
@@ -13659,8 +14015,10 @@
       <c r="H442" s="18" t="inlineStr"/>
       <c r="I442" s="18" t="inlineStr"/>
       <c r="J442" s="18" t="inlineStr"/>
-      <c r="K442" s="22" t="n">
-        <v>250</v>
+      <c r="K442" s="22" t="inlineStr">
+        <is>
+          <t>250</t>
+        </is>
       </c>
       <c r="L442" s="18" t="inlineStr">
         <is>
@@ -13687,8 +14045,10 @@
       <c r="H443" s="18" t="inlineStr"/>
       <c r="I443" s="18" t="inlineStr"/>
       <c r="J443" s="18" t="inlineStr"/>
-      <c r="K443" s="22" t="n">
-        <v>416</v>
+      <c r="K443" s="22" t="inlineStr">
+        <is>
+          <t>416</t>
+        </is>
       </c>
       <c r="L443" s="18" t="inlineStr">
         <is>
@@ -13715,8 +14075,10 @@
       <c r="H444" s="18" t="inlineStr"/>
       <c r="I444" s="18" t="inlineStr"/>
       <c r="J444" s="18" t="inlineStr"/>
-      <c r="K444" s="22" t="n">
-        <v>587</v>
+      <c r="K444" s="22" t="inlineStr">
+        <is>
+          <t>587</t>
+        </is>
       </c>
       <c r="L444" s="18" t="inlineStr">
         <is>
@@ -13743,8 +14105,10 @@
       <c r="H445" s="18" t="inlineStr"/>
       <c r="I445" s="18" t="inlineStr"/>
       <c r="J445" s="18" t="inlineStr"/>
-      <c r="K445" s="22" t="n">
-        <v>250</v>
+      <c r="K445" s="22" t="inlineStr">
+        <is>
+          <t>250</t>
+        </is>
       </c>
       <c r="L445" s="18" t="inlineStr">
         <is>
@@ -13771,8 +14135,10 @@
       <c r="H446" s="18" t="inlineStr"/>
       <c r="I446" s="18" t="inlineStr"/>
       <c r="J446" s="18" t="inlineStr"/>
-      <c r="K446" s="22" t="n">
-        <v>2297</v>
+      <c r="K446" s="22" t="inlineStr">
+        <is>
+          <t>2297</t>
+        </is>
       </c>
       <c r="L446" s="18" t="inlineStr">
         <is>
@@ -13799,8 +14165,10 @@
       <c r="H447" s="18" t="inlineStr"/>
       <c r="I447" s="18" t="inlineStr"/>
       <c r="J447" s="18" t="inlineStr"/>
-      <c r="K447" s="22" t="n">
-        <v>750</v>
+      <c r="K447" s="22" t="inlineStr">
+        <is>
+          <t>750</t>
+        </is>
       </c>
       <c r="L447" s="18" t="inlineStr">
         <is>
@@ -13827,8 +14195,10 @@
       <c r="H448" s="18" t="inlineStr"/>
       <c r="I448" s="18" t="inlineStr"/>
       <c r="J448" s="18" t="inlineStr"/>
-      <c r="K448" s="22" t="n">
-        <v>27408</v>
+      <c r="K448" s="22" t="inlineStr">
+        <is>
+          <t>27408</t>
+        </is>
       </c>
       <c r="L448" s="18" t="inlineStr">
         <is>
@@ -13855,8 +14225,10 @@
       <c r="H449" s="18" t="inlineStr"/>
       <c r="I449" s="18" t="inlineStr"/>
       <c r="J449" s="18" t="inlineStr"/>
-      <c r="K449" s="22" t="n">
-        <v>2500</v>
+      <c r="K449" s="22" t="inlineStr">
+        <is>
+          <t>2500</t>
+        </is>
       </c>
       <c r="L449" s="18" t="inlineStr">
         <is>
@@ -13883,8 +14255,10 @@
       <c r="H450" s="18" t="inlineStr"/>
       <c r="I450" s="18" t="inlineStr"/>
       <c r="J450" s="18" t="inlineStr"/>
-      <c r="K450" s="22" t="n">
-        <v>416</v>
+      <c r="K450" s="22" t="inlineStr">
+        <is>
+          <t>416</t>
+        </is>
       </c>
       <c r="L450" s="18" t="inlineStr">
         <is>
@@ -13911,8 +14285,10 @@
       <c r="H451" s="18" t="inlineStr"/>
       <c r="I451" s="18" t="inlineStr"/>
       <c r="J451" s="18" t="inlineStr"/>
-      <c r="K451" s="22" t="n">
-        <v>1826</v>
+      <c r="K451" s="22" t="inlineStr">
+        <is>
+          <t>1826</t>
+        </is>
       </c>
       <c r="L451" s="18" t="inlineStr">
         <is>
@@ -13939,8 +14315,10 @@
       <c r="H452" s="18" t="inlineStr"/>
       <c r="I452" s="18" t="inlineStr"/>
       <c r="J452" s="18" t="inlineStr"/>
-      <c r="K452" s="22" t="n">
-        <v>23812</v>
+      <c r="K452" s="22" t="inlineStr">
+        <is>
+          <t>23812</t>
+        </is>
       </c>
       <c r="L452" s="18" t="inlineStr">
         <is>
@@ -13967,8 +14345,10 @@
       <c r="H453" s="18" t="inlineStr"/>
       <c r="I453" s="18" t="inlineStr"/>
       <c r="J453" s="18" t="inlineStr"/>
-      <c r="K453" s="22" t="n">
-        <v>1250</v>
+      <c r="K453" s="22" t="inlineStr">
+        <is>
+          <t>1250</t>
+        </is>
       </c>
       <c r="L453" s="18" t="inlineStr">
         <is>
@@ -13995,8 +14375,10 @@
       <c r="H454" s="18" t="inlineStr"/>
       <c r="I454" s="18" t="inlineStr"/>
       <c r="J454" s="18" t="inlineStr"/>
-      <c r="K454" s="22" t="n">
-        <v>53301</v>
+      <c r="K454" s="22" t="inlineStr">
+        <is>
+          <t>53301</t>
+        </is>
       </c>
       <c r="L454" s="18" t="inlineStr">
         <is>
@@ -14023,8 +14405,10 @@
       <c r="H455" s="18" t="inlineStr"/>
       <c r="I455" s="18" t="inlineStr"/>
       <c r="J455" s="18" t="inlineStr"/>
-      <c r="K455" s="22" t="n">
-        <v>2500</v>
+      <c r="K455" s="22" t="inlineStr">
+        <is>
+          <t>2500</t>
+        </is>
       </c>
       <c r="L455" s="18" t="inlineStr">
         <is>
@@ -14051,8 +14435,10 @@
       <c r="H456" s="18" t="inlineStr"/>
       <c r="I456" s="18" t="inlineStr"/>
       <c r="J456" s="18" t="inlineStr"/>
-      <c r="K456" s="22" t="n">
-        <v>2116</v>
+      <c r="K456" s="22" t="inlineStr">
+        <is>
+          <t>2116</t>
+        </is>
       </c>
       <c r="L456" s="18" t="inlineStr">
         <is>
@@ -14079,8 +14465,10 @@
       <c r="H457" s="18" t="inlineStr"/>
       <c r="I457" s="18" t="inlineStr"/>
       <c r="J457" s="18" t="inlineStr"/>
-      <c r="K457" s="22" t="n">
-        <v>250</v>
+      <c r="K457" s="22" t="inlineStr">
+        <is>
+          <t>250</t>
+        </is>
       </c>
       <c r="L457" s="18" t="inlineStr">
         <is>
@@ -14107,8 +14495,10 @@
       <c r="H458" s="18" t="inlineStr"/>
       <c r="I458" s="18" t="inlineStr"/>
       <c r="J458" s="18" t="inlineStr"/>
-      <c r="K458" s="22" t="n">
-        <v>6060</v>
+      <c r="K458" s="22" t="inlineStr">
+        <is>
+          <t>6060</t>
+        </is>
       </c>
       <c r="L458" s="18" t="inlineStr">
         <is>
@@ -14135,8 +14525,10 @@
       <c r="H459" s="18" t="inlineStr"/>
       <c r="I459" s="18" t="inlineStr"/>
       <c r="J459" s="18" t="inlineStr"/>
-      <c r="K459" s="22" t="n">
-        <v>104540</v>
+      <c r="K459" s="22" t="inlineStr">
+        <is>
+          <t>104540</t>
+        </is>
       </c>
       <c r="L459" s="18" t="inlineStr">
         <is>
@@ -14163,8 +14555,10 @@
       <c r="H460" s="18" t="inlineStr"/>
       <c r="I460" s="18" t="inlineStr"/>
       <c r="J460" s="18" t="inlineStr"/>
-      <c r="K460" s="22" t="n">
-        <v>104540</v>
+      <c r="K460" s="22" t="inlineStr">
+        <is>
+          <t>104540</t>
+        </is>
       </c>
       <c r="L460" s="18" t="inlineStr">
         <is>
@@ -14191,8 +14585,10 @@
       <c r="H461" s="18" t="inlineStr"/>
       <c r="I461" s="18" t="inlineStr"/>
       <c r="J461" s="18" t="inlineStr"/>
-      <c r="K461" s="22" t="n">
-        <v>68357</v>
+      <c r="K461" s="22" t="inlineStr">
+        <is>
+          <t>68357</t>
+        </is>
       </c>
       <c r="L461" s="18" t="inlineStr">
         <is>
@@ -14219,8 +14615,10 @@
       <c r="H462" s="18" t="inlineStr"/>
       <c r="I462" s="18" t="inlineStr"/>
       <c r="J462" s="18" t="inlineStr"/>
-      <c r="K462" s="22" t="n">
-        <v>3218390</v>
+      <c r="K462" s="22" t="inlineStr">
+        <is>
+          <t>3218390</t>
+        </is>
       </c>
       <c r="L462" s="18" t="inlineStr">
         <is>
@@ -14295,16 +14693,20 @@
       <c r="B465" s="2" t="inlineStr"/>
       <c r="C465" s="1" t="inlineStr"/>
       <c r="D465" s="1" t="inlineStr"/>
-      <c r="E465" s="2" t="n">
-        <v>3782051767.82</v>
+      <c r="E465" s="2" t="inlineStr">
+        <is>
+          <t>3782051767.82</t>
+        </is>
       </c>
       <c r="F465" s="1" t="inlineStr"/>
       <c r="G465" s="1" t="inlineStr"/>
       <c r="H465" s="1" t="inlineStr"/>
       <c r="I465" s="1" t="inlineStr"/>
       <c r="J465" s="1" t="inlineStr"/>
-      <c r="K465" s="25" t="n">
-        <v>144741173.97</v>
+      <c r="K465" s="25" t="inlineStr">
+        <is>
+          <t>144741173.97</t>
+        </is>
       </c>
       <c r="L465" s="1" t="inlineStr"/>
     </row>
@@ -14327,8 +14729,10 @@
       <c r="H466" s="1" t="inlineStr"/>
       <c r="I466" s="1" t="inlineStr"/>
       <c r="J466" s="1" t="inlineStr"/>
-      <c r="K466" s="25" t="n">
-        <v>3637310593.85</v>
+      <c r="K466" s="25" t="inlineStr">
+        <is>
+          <t>3637310593.85</t>
+        </is>
       </c>
       <c r="L466" s="1" t="inlineStr"/>
     </row>
@@ -14337,16 +14741,20 @@
       <c r="B467" s="2" t="inlineStr"/>
       <c r="C467" s="1" t="inlineStr"/>
       <c r="D467" s="1" t="inlineStr"/>
-      <c r="E467" s="2" t="n">
-        <v>3782051767.82</v>
+      <c r="E467" s="2" t="inlineStr">
+        <is>
+          <t>3782051767.82</t>
+        </is>
       </c>
       <c r="F467" s="1" t="inlineStr"/>
       <c r="G467" s="1" t="inlineStr"/>
       <c r="H467" s="1" t="inlineStr"/>
       <c r="I467" s="1" t="inlineStr"/>
       <c r="J467" s="1" t="inlineStr"/>
-      <c r="K467" s="25" t="n">
-        <v>3782051767.82</v>
+      <c r="K467" s="25" t="inlineStr">
+        <is>
+          <t>3782051767.82</t>
+        </is>
       </c>
       <c r="L467" s="1" t="inlineStr"/>
     </row>

</xml_diff>